<commit_message>
MAJ JDT + Problèmes.docx 12.06.17
</commit_message>
<xml_diff>
--- a/doc/DemoMotJDT-pittierfa.xlsx
+++ b/doc/DemoMotJDT-pittierfa.xlsx
@@ -36,7 +36,7 @@
     <definedName name="objRealizedWeek" localSheetId="7">JNLTRAV!$A$1:$D$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Diagramme!$A$1:$PT$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$306</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$309</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Planning!$A$1:$D$224</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="129">
   <si>
     <t>Module :</t>
   </si>
@@ -418,6 +418,42 @@
   </si>
   <si>
     <t>Commit modifications du jour (Site + JDT + mise à jour daily scrum)</t>
+  </si>
+  <si>
+    <t>Push de la branche dev car le dernier commit était uniquement en local (checkout de la branche pour pouvoir faire le push), Jimmy récupère site mais il lui manque bdd -&gt; passe sur K du groupe</t>
+  </si>
+  <si>
+    <t>que 4 périodes lundi matin</t>
+  </si>
+  <si>
+    <t>https://github.com/FriendsOfTYPO3/extension_builder/tree/8.6</t>
+  </si>
+  <si>
+    <t>https://github.com/TYPO3-extensions/extension_builder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Met en place une extension mais avant de la sauvegarder remarque que nous avons extension builder pour une version trop vieille de typo3 (On a téléchargé sur mauvais depo). </t>
+  </si>
+  <si>
+    <t>On va demander à mme hardeger qui nous montre que nous avons mauvaise version et où télécharger la dernière version (depot github)</t>
+  </si>
+  <si>
+    <t>On n'avait pas très bien compris s'il fallait mettre en place un frontend et quelle cardinalité il fallait mettre -&gt; montre un bon doccument à lire pour nous aider</t>
+  </si>
+  <si>
+    <t>Avec Jimmy regarde quels propriétés nous avons besoin pour notre extension et recommence à créer notre extension</t>
+  </si>
+  <si>
+    <t>Terminé création de l'extension</t>
+  </si>
+  <si>
+    <t>Règle un petit bogue: Lorsqu'on est connecté, doit plus voir la page "connexion" dans le nav</t>
+  </si>
+  <si>
+    <t>(Commit pour les branches FPR02 et DEV01 mais checkout entre les branches long car DEV01 contient tout typo3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise au propre du doccument </t>
   </si>
 </sst>
 </file>
@@ -1592,12 +1628,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1606,6 +1636,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3375,27 +3411,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId4" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId4" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3425,27 +3461,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId8" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId8" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3483,470 +3519,470 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="123" t="s">
+      <c r="D2" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
-      <c r="Y2" s="124"/>
-      <c r="Z2" s="124"/>
-      <c r="AA2" s="124"/>
-      <c r="AB2" s="124"/>
-      <c r="AC2" s="124"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="123" t="s">
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="122"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="122"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="122"/>
+      <c r="AA2" s="122"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="122"/>
+      <c r="AD2" s="123"/>
+      <c r="AE2" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="124"/>
-      <c r="AG2" s="124"/>
-      <c r="AH2" s="124"/>
-      <c r="AI2" s="124"/>
-      <c r="AJ2" s="124"/>
-      <c r="AK2" s="124"/>
-      <c r="AL2" s="124"/>
-      <c r="AM2" s="124"/>
-      <c r="AN2" s="124"/>
-      <c r="AO2" s="124"/>
-      <c r="AP2" s="124"/>
-      <c r="AQ2" s="124"/>
-      <c r="AR2" s="124"/>
-      <c r="AS2" s="124"/>
-      <c r="AT2" s="124"/>
-      <c r="AU2" s="124"/>
-      <c r="AV2" s="124"/>
-      <c r="AW2" s="124"/>
-      <c r="AX2" s="124"/>
-      <c r="AY2" s="124"/>
-      <c r="AZ2" s="124"/>
-      <c r="BA2" s="124"/>
-      <c r="BB2" s="124"/>
-      <c r="BC2" s="124"/>
-      <c r="BD2" s="124"/>
-      <c r="BE2" s="125"/>
-      <c r="BF2" s="123" t="s">
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="122"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="122"/>
+      <c r="AK2" s="122"/>
+      <c r="AL2" s="122"/>
+      <c r="AM2" s="122"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="122"/>
+      <c r="AP2" s="122"/>
+      <c r="AQ2" s="122"/>
+      <c r="AR2" s="122"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="122"/>
+      <c r="AU2" s="122"/>
+      <c r="AV2" s="122"/>
+      <c r="AW2" s="122"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="122"/>
+      <c r="AZ2" s="122"/>
+      <c r="BA2" s="122"/>
+      <c r="BB2" s="122"/>
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="123"/>
+      <c r="BF2" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="BG2" s="124"/>
-      <c r="BH2" s="124"/>
-      <c r="BI2" s="124"/>
-      <c r="BJ2" s="124"/>
-      <c r="BK2" s="124"/>
-      <c r="BL2" s="124"/>
-      <c r="BM2" s="124"/>
-      <c r="BN2" s="124"/>
-      <c r="BO2" s="124"/>
-      <c r="BP2" s="124"/>
-      <c r="BQ2" s="124"/>
-      <c r="BR2" s="124"/>
-      <c r="BS2" s="124"/>
-      <c r="BT2" s="124"/>
-      <c r="BU2" s="124"/>
-      <c r="BV2" s="124"/>
-      <c r="BW2" s="124"/>
-      <c r="BX2" s="124"/>
-      <c r="BY2" s="124"/>
-      <c r="BZ2" s="124"/>
-      <c r="CA2" s="124"/>
-      <c r="CB2" s="124"/>
-      <c r="CC2" s="124"/>
-      <c r="CD2" s="124"/>
-      <c r="CE2" s="124"/>
-      <c r="CF2" s="125"/>
-      <c r="CG2" s="123" t="s">
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="122"/>
+      <c r="BQ2" s="122"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="122"/>
+      <c r="BV2" s="122"/>
+      <c r="BW2" s="122"/>
+      <c r="BX2" s="122"/>
+      <c r="BY2" s="122"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="122"/>
+      <c r="CB2" s="122"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="122"/>
+      <c r="CE2" s="122"/>
+      <c r="CF2" s="123"/>
+      <c r="CG2" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="CH2" s="124"/>
-      <c r="CI2" s="124"/>
-      <c r="CJ2" s="124"/>
-      <c r="CK2" s="124"/>
-      <c r="CL2" s="124"/>
-      <c r="CM2" s="124"/>
-      <c r="CN2" s="124"/>
-      <c r="CO2" s="124"/>
-      <c r="CP2" s="124"/>
-      <c r="CQ2" s="124"/>
-      <c r="CR2" s="124"/>
-      <c r="CS2" s="124"/>
-      <c r="CT2" s="124"/>
-      <c r="CU2" s="124"/>
-      <c r="CV2" s="124"/>
-      <c r="CW2" s="124"/>
-      <c r="CX2" s="124"/>
-      <c r="CY2" s="124"/>
-      <c r="CZ2" s="124"/>
-      <c r="DA2" s="124"/>
-      <c r="DB2" s="124"/>
-      <c r="DC2" s="124"/>
-      <c r="DD2" s="124"/>
-      <c r="DE2" s="124"/>
-      <c r="DF2" s="124"/>
-      <c r="DG2" s="125"/>
-      <c r="DH2" s="123" t="s">
+      <c r="CH2" s="122"/>
+      <c r="CI2" s="122"/>
+      <c r="CJ2" s="122"/>
+      <c r="CK2" s="122"/>
+      <c r="CL2" s="122"/>
+      <c r="CM2" s="122"/>
+      <c r="CN2" s="122"/>
+      <c r="CO2" s="122"/>
+      <c r="CP2" s="122"/>
+      <c r="CQ2" s="122"/>
+      <c r="CR2" s="122"/>
+      <c r="CS2" s="122"/>
+      <c r="CT2" s="122"/>
+      <c r="CU2" s="122"/>
+      <c r="CV2" s="122"/>
+      <c r="CW2" s="122"/>
+      <c r="CX2" s="122"/>
+      <c r="CY2" s="122"/>
+      <c r="CZ2" s="122"/>
+      <c r="DA2" s="122"/>
+      <c r="DB2" s="122"/>
+      <c r="DC2" s="122"/>
+      <c r="DD2" s="122"/>
+      <c r="DE2" s="122"/>
+      <c r="DF2" s="122"/>
+      <c r="DG2" s="123"/>
+      <c r="DH2" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="DI2" s="124"/>
-      <c r="DJ2" s="124"/>
-      <c r="DK2" s="124"/>
-      <c r="DL2" s="124"/>
-      <c r="DM2" s="124"/>
-      <c r="DN2" s="124"/>
-      <c r="DO2" s="124"/>
-      <c r="DP2" s="124"/>
-      <c r="DQ2" s="124"/>
-      <c r="DR2" s="124"/>
-      <c r="DS2" s="124"/>
-      <c r="DT2" s="124"/>
-      <c r="DU2" s="124"/>
-      <c r="DV2" s="124"/>
-      <c r="DW2" s="124"/>
-      <c r="DX2" s="124"/>
-      <c r="DY2" s="124"/>
-      <c r="DZ2" s="124"/>
-      <c r="EA2" s="124"/>
-      <c r="EB2" s="124"/>
-      <c r="EC2" s="124"/>
-      <c r="ED2" s="124"/>
-      <c r="EE2" s="124"/>
-      <c r="EF2" s="124"/>
-      <c r="EG2" s="124"/>
-      <c r="EH2" s="125"/>
-      <c r="EI2" s="123" t="s">
+      <c r="DI2" s="122"/>
+      <c r="DJ2" s="122"/>
+      <c r="DK2" s="122"/>
+      <c r="DL2" s="122"/>
+      <c r="DM2" s="122"/>
+      <c r="DN2" s="122"/>
+      <c r="DO2" s="122"/>
+      <c r="DP2" s="122"/>
+      <c r="DQ2" s="122"/>
+      <c r="DR2" s="122"/>
+      <c r="DS2" s="122"/>
+      <c r="DT2" s="122"/>
+      <c r="DU2" s="122"/>
+      <c r="DV2" s="122"/>
+      <c r="DW2" s="122"/>
+      <c r="DX2" s="122"/>
+      <c r="DY2" s="122"/>
+      <c r="DZ2" s="122"/>
+      <c r="EA2" s="122"/>
+      <c r="EB2" s="122"/>
+      <c r="EC2" s="122"/>
+      <c r="ED2" s="122"/>
+      <c r="EE2" s="122"/>
+      <c r="EF2" s="122"/>
+      <c r="EG2" s="122"/>
+      <c r="EH2" s="123"/>
+      <c r="EI2" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="EJ2" s="124"/>
-      <c r="EK2" s="124"/>
-      <c r="EL2" s="124"/>
-      <c r="EM2" s="124"/>
-      <c r="EN2" s="124"/>
-      <c r="EO2" s="124"/>
-      <c r="EP2" s="124"/>
-      <c r="EQ2" s="124"/>
-      <c r="ER2" s="124"/>
-      <c r="ES2" s="124"/>
-      <c r="ET2" s="124"/>
-      <c r="EU2" s="124"/>
-      <c r="EV2" s="124"/>
-      <c r="EW2" s="124"/>
-      <c r="EX2" s="124"/>
-      <c r="EY2" s="124"/>
-      <c r="EZ2" s="124"/>
-      <c r="FA2" s="124"/>
-      <c r="FB2" s="124"/>
-      <c r="FC2" s="124"/>
-      <c r="FD2" s="124"/>
-      <c r="FE2" s="124"/>
-      <c r="FF2" s="124"/>
-      <c r="FG2" s="124"/>
-      <c r="FH2" s="124"/>
-      <c r="FI2" s="125"/>
-      <c r="FJ2" s="123" t="s">
+      <c r="EJ2" s="122"/>
+      <c r="EK2" s="122"/>
+      <c r="EL2" s="122"/>
+      <c r="EM2" s="122"/>
+      <c r="EN2" s="122"/>
+      <c r="EO2" s="122"/>
+      <c r="EP2" s="122"/>
+      <c r="EQ2" s="122"/>
+      <c r="ER2" s="122"/>
+      <c r="ES2" s="122"/>
+      <c r="ET2" s="122"/>
+      <c r="EU2" s="122"/>
+      <c r="EV2" s="122"/>
+      <c r="EW2" s="122"/>
+      <c r="EX2" s="122"/>
+      <c r="EY2" s="122"/>
+      <c r="EZ2" s="122"/>
+      <c r="FA2" s="122"/>
+      <c r="FB2" s="122"/>
+      <c r="FC2" s="122"/>
+      <c r="FD2" s="122"/>
+      <c r="FE2" s="122"/>
+      <c r="FF2" s="122"/>
+      <c r="FG2" s="122"/>
+      <c r="FH2" s="122"/>
+      <c r="FI2" s="123"/>
+      <c r="FJ2" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="FK2" s="124"/>
-      <c r="FL2" s="124"/>
-      <c r="FM2" s="124"/>
-      <c r="FN2" s="124"/>
-      <c r="FO2" s="124"/>
-      <c r="FP2" s="124"/>
-      <c r="FQ2" s="124"/>
-      <c r="FR2" s="124"/>
-      <c r="FS2" s="124"/>
-      <c r="FT2" s="124"/>
-      <c r="FU2" s="124"/>
-      <c r="FV2" s="124"/>
-      <c r="FW2" s="124"/>
-      <c r="FX2" s="124"/>
-      <c r="FY2" s="124"/>
-      <c r="FZ2" s="124"/>
-      <c r="GA2" s="124"/>
-      <c r="GB2" s="124"/>
-      <c r="GC2" s="124"/>
-      <c r="GD2" s="124"/>
-      <c r="GE2" s="124"/>
-      <c r="GF2" s="124"/>
-      <c r="GG2" s="124"/>
-      <c r="GH2" s="124"/>
-      <c r="GI2" s="124"/>
-      <c r="GJ2" s="125"/>
-      <c r="GK2" s="123" t="s">
+      <c r="FK2" s="122"/>
+      <c r="FL2" s="122"/>
+      <c r="FM2" s="122"/>
+      <c r="FN2" s="122"/>
+      <c r="FO2" s="122"/>
+      <c r="FP2" s="122"/>
+      <c r="FQ2" s="122"/>
+      <c r="FR2" s="122"/>
+      <c r="FS2" s="122"/>
+      <c r="FT2" s="122"/>
+      <c r="FU2" s="122"/>
+      <c r="FV2" s="122"/>
+      <c r="FW2" s="122"/>
+      <c r="FX2" s="122"/>
+      <c r="FY2" s="122"/>
+      <c r="FZ2" s="122"/>
+      <c r="GA2" s="122"/>
+      <c r="GB2" s="122"/>
+      <c r="GC2" s="122"/>
+      <c r="GD2" s="122"/>
+      <c r="GE2" s="122"/>
+      <c r="GF2" s="122"/>
+      <c r="GG2" s="122"/>
+      <c r="GH2" s="122"/>
+      <c r="GI2" s="122"/>
+      <c r="GJ2" s="123"/>
+      <c r="GK2" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="GL2" s="124"/>
-      <c r="GM2" s="124"/>
-      <c r="GN2" s="124"/>
-      <c r="GO2" s="124"/>
-      <c r="GP2" s="124"/>
-      <c r="GQ2" s="124"/>
-      <c r="GR2" s="124"/>
-      <c r="GS2" s="124"/>
-      <c r="GT2" s="124"/>
-      <c r="GU2" s="124"/>
-      <c r="GV2" s="124"/>
-      <c r="GW2" s="124"/>
-      <c r="GX2" s="124"/>
-      <c r="GY2" s="124"/>
-      <c r="GZ2" s="124"/>
-      <c r="HA2" s="124"/>
-      <c r="HB2" s="124"/>
-      <c r="HC2" s="124"/>
-      <c r="HD2" s="124"/>
-      <c r="HE2" s="124"/>
-      <c r="HF2" s="124"/>
-      <c r="HG2" s="124"/>
-      <c r="HH2" s="124"/>
-      <c r="HI2" s="124"/>
-      <c r="HJ2" s="124"/>
-      <c r="HK2" s="125"/>
-      <c r="HL2" s="123" t="s">
+      <c r="GL2" s="122"/>
+      <c r="GM2" s="122"/>
+      <c r="GN2" s="122"/>
+      <c r="GO2" s="122"/>
+      <c r="GP2" s="122"/>
+      <c r="GQ2" s="122"/>
+      <c r="GR2" s="122"/>
+      <c r="GS2" s="122"/>
+      <c r="GT2" s="122"/>
+      <c r="GU2" s="122"/>
+      <c r="GV2" s="122"/>
+      <c r="GW2" s="122"/>
+      <c r="GX2" s="122"/>
+      <c r="GY2" s="122"/>
+      <c r="GZ2" s="122"/>
+      <c r="HA2" s="122"/>
+      <c r="HB2" s="122"/>
+      <c r="HC2" s="122"/>
+      <c r="HD2" s="122"/>
+      <c r="HE2" s="122"/>
+      <c r="HF2" s="122"/>
+      <c r="HG2" s="122"/>
+      <c r="HH2" s="122"/>
+      <c r="HI2" s="122"/>
+      <c r="HJ2" s="122"/>
+      <c r="HK2" s="123"/>
+      <c r="HL2" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="HM2" s="124"/>
-      <c r="HN2" s="124"/>
-      <c r="HO2" s="124"/>
-      <c r="HP2" s="124"/>
-      <c r="HQ2" s="124"/>
-      <c r="HR2" s="124"/>
-      <c r="HS2" s="124"/>
-      <c r="HT2" s="124"/>
-      <c r="HU2" s="124"/>
-      <c r="HV2" s="124"/>
-      <c r="HW2" s="124"/>
-      <c r="HX2" s="124"/>
-      <c r="HY2" s="124"/>
-      <c r="HZ2" s="124"/>
-      <c r="IA2" s="124"/>
-      <c r="IB2" s="124"/>
-      <c r="IC2" s="124"/>
-      <c r="ID2" s="124"/>
-      <c r="IE2" s="124"/>
-      <c r="IF2" s="124"/>
-      <c r="IG2" s="124"/>
-      <c r="IH2" s="124"/>
-      <c r="II2" s="124"/>
-      <c r="IJ2" s="124"/>
-      <c r="IK2" s="124"/>
-      <c r="IL2" s="125"/>
-      <c r="IM2" s="123" t="s">
+      <c r="HM2" s="122"/>
+      <c r="HN2" s="122"/>
+      <c r="HO2" s="122"/>
+      <c r="HP2" s="122"/>
+      <c r="HQ2" s="122"/>
+      <c r="HR2" s="122"/>
+      <c r="HS2" s="122"/>
+      <c r="HT2" s="122"/>
+      <c r="HU2" s="122"/>
+      <c r="HV2" s="122"/>
+      <c r="HW2" s="122"/>
+      <c r="HX2" s="122"/>
+      <c r="HY2" s="122"/>
+      <c r="HZ2" s="122"/>
+      <c r="IA2" s="122"/>
+      <c r="IB2" s="122"/>
+      <c r="IC2" s="122"/>
+      <c r="ID2" s="122"/>
+      <c r="IE2" s="122"/>
+      <c r="IF2" s="122"/>
+      <c r="IG2" s="122"/>
+      <c r="IH2" s="122"/>
+      <c r="II2" s="122"/>
+      <c r="IJ2" s="122"/>
+      <c r="IK2" s="122"/>
+      <c r="IL2" s="123"/>
+      <c r="IM2" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="IN2" s="124"/>
-      <c r="IO2" s="124"/>
-      <c r="IP2" s="124"/>
-      <c r="IQ2" s="124"/>
-      <c r="IR2" s="124"/>
-      <c r="IS2" s="124"/>
-      <c r="IT2" s="124"/>
-      <c r="IU2" s="124"/>
-      <c r="IV2" s="124"/>
-      <c r="IW2" s="124"/>
-      <c r="IX2" s="124"/>
-      <c r="IY2" s="124"/>
-      <c r="IZ2" s="124"/>
-      <c r="JA2" s="124"/>
-      <c r="JB2" s="124"/>
-      <c r="JC2" s="124"/>
-      <c r="JD2" s="124"/>
-      <c r="JE2" s="124"/>
-      <c r="JF2" s="124"/>
-      <c r="JG2" s="124"/>
-      <c r="JH2" s="124"/>
-      <c r="JI2" s="124"/>
-      <c r="JJ2" s="124"/>
-      <c r="JK2" s="124"/>
-      <c r="JL2" s="124"/>
-      <c r="JM2" s="125"/>
-      <c r="JN2" s="123" t="s">
+      <c r="IN2" s="122"/>
+      <c r="IO2" s="122"/>
+      <c r="IP2" s="122"/>
+      <c r="IQ2" s="122"/>
+      <c r="IR2" s="122"/>
+      <c r="IS2" s="122"/>
+      <c r="IT2" s="122"/>
+      <c r="IU2" s="122"/>
+      <c r="IV2" s="122"/>
+      <c r="IW2" s="122"/>
+      <c r="IX2" s="122"/>
+      <c r="IY2" s="122"/>
+      <c r="IZ2" s="122"/>
+      <c r="JA2" s="122"/>
+      <c r="JB2" s="122"/>
+      <c r="JC2" s="122"/>
+      <c r="JD2" s="122"/>
+      <c r="JE2" s="122"/>
+      <c r="JF2" s="122"/>
+      <c r="JG2" s="122"/>
+      <c r="JH2" s="122"/>
+      <c r="JI2" s="122"/>
+      <c r="JJ2" s="122"/>
+      <c r="JK2" s="122"/>
+      <c r="JL2" s="122"/>
+      <c r="JM2" s="123"/>
+      <c r="JN2" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="JO2" s="124"/>
-      <c r="JP2" s="124"/>
-      <c r="JQ2" s="124"/>
-      <c r="JR2" s="124"/>
-      <c r="JS2" s="124"/>
-      <c r="JT2" s="124"/>
-      <c r="JU2" s="124"/>
-      <c r="JV2" s="124"/>
-      <c r="JW2" s="124"/>
-      <c r="JX2" s="124"/>
-      <c r="JY2" s="124"/>
-      <c r="JZ2" s="124"/>
-      <c r="KA2" s="124"/>
-      <c r="KB2" s="124"/>
-      <c r="KC2" s="124"/>
-      <c r="KD2" s="124"/>
-      <c r="KE2" s="124"/>
-      <c r="KF2" s="124"/>
-      <c r="KG2" s="124"/>
-      <c r="KH2" s="124"/>
-      <c r="KI2" s="124"/>
-      <c r="KJ2" s="124"/>
-      <c r="KK2" s="124"/>
-      <c r="KL2" s="124"/>
-      <c r="KM2" s="124"/>
-      <c r="KN2" s="125"/>
-      <c r="KO2" s="123" t="s">
+      <c r="JO2" s="122"/>
+      <c r="JP2" s="122"/>
+      <c r="JQ2" s="122"/>
+      <c r="JR2" s="122"/>
+      <c r="JS2" s="122"/>
+      <c r="JT2" s="122"/>
+      <c r="JU2" s="122"/>
+      <c r="JV2" s="122"/>
+      <c r="JW2" s="122"/>
+      <c r="JX2" s="122"/>
+      <c r="JY2" s="122"/>
+      <c r="JZ2" s="122"/>
+      <c r="KA2" s="122"/>
+      <c r="KB2" s="122"/>
+      <c r="KC2" s="122"/>
+      <c r="KD2" s="122"/>
+      <c r="KE2" s="122"/>
+      <c r="KF2" s="122"/>
+      <c r="KG2" s="122"/>
+      <c r="KH2" s="122"/>
+      <c r="KI2" s="122"/>
+      <c r="KJ2" s="122"/>
+      <c r="KK2" s="122"/>
+      <c r="KL2" s="122"/>
+      <c r="KM2" s="122"/>
+      <c r="KN2" s="123"/>
+      <c r="KO2" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="KP2" s="124"/>
-      <c r="KQ2" s="124"/>
-      <c r="KR2" s="124"/>
-      <c r="KS2" s="124"/>
-      <c r="KT2" s="124"/>
-      <c r="KU2" s="124"/>
-      <c r="KV2" s="124"/>
-      <c r="KW2" s="124"/>
-      <c r="KX2" s="124"/>
-      <c r="KY2" s="124"/>
-      <c r="KZ2" s="124"/>
-      <c r="LA2" s="124"/>
-      <c r="LB2" s="124"/>
-      <c r="LC2" s="124"/>
-      <c r="LD2" s="124"/>
-      <c r="LE2" s="124"/>
-      <c r="LF2" s="124"/>
-      <c r="LG2" s="124"/>
-      <c r="LH2" s="124"/>
-      <c r="LI2" s="124"/>
-      <c r="LJ2" s="124"/>
-      <c r="LK2" s="124"/>
-      <c r="LL2" s="124"/>
-      <c r="LM2" s="124"/>
-      <c r="LN2" s="124"/>
-      <c r="LO2" s="125"/>
-      <c r="LP2" s="123" t="s">
+      <c r="KP2" s="122"/>
+      <c r="KQ2" s="122"/>
+      <c r="KR2" s="122"/>
+      <c r="KS2" s="122"/>
+      <c r="KT2" s="122"/>
+      <c r="KU2" s="122"/>
+      <c r="KV2" s="122"/>
+      <c r="KW2" s="122"/>
+      <c r="KX2" s="122"/>
+      <c r="KY2" s="122"/>
+      <c r="KZ2" s="122"/>
+      <c r="LA2" s="122"/>
+      <c r="LB2" s="122"/>
+      <c r="LC2" s="122"/>
+      <c r="LD2" s="122"/>
+      <c r="LE2" s="122"/>
+      <c r="LF2" s="122"/>
+      <c r="LG2" s="122"/>
+      <c r="LH2" s="122"/>
+      <c r="LI2" s="122"/>
+      <c r="LJ2" s="122"/>
+      <c r="LK2" s="122"/>
+      <c r="LL2" s="122"/>
+      <c r="LM2" s="122"/>
+      <c r="LN2" s="122"/>
+      <c r="LO2" s="123"/>
+      <c r="LP2" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="LQ2" s="124"/>
-      <c r="LR2" s="124"/>
-      <c r="LS2" s="124"/>
-      <c r="LT2" s="124"/>
-      <c r="LU2" s="124"/>
-      <c r="LV2" s="124"/>
-      <c r="LW2" s="124"/>
-      <c r="LX2" s="124"/>
-      <c r="LY2" s="124"/>
-      <c r="LZ2" s="124"/>
-      <c r="MA2" s="124"/>
-      <c r="MB2" s="124"/>
-      <c r="MC2" s="124"/>
-      <c r="MD2" s="124"/>
-      <c r="ME2" s="124"/>
-      <c r="MF2" s="124"/>
-      <c r="MG2" s="124"/>
-      <c r="MH2" s="124"/>
-      <c r="MI2" s="124"/>
-      <c r="MJ2" s="124"/>
-      <c r="MK2" s="124"/>
-      <c r="ML2" s="124"/>
-      <c r="MM2" s="124"/>
-      <c r="MN2" s="124"/>
-      <c r="MO2" s="124"/>
-      <c r="MP2" s="125"/>
-      <c r="MQ2" s="123" t="s">
+      <c r="LQ2" s="122"/>
+      <c r="LR2" s="122"/>
+      <c r="LS2" s="122"/>
+      <c r="LT2" s="122"/>
+      <c r="LU2" s="122"/>
+      <c r="LV2" s="122"/>
+      <c r="LW2" s="122"/>
+      <c r="LX2" s="122"/>
+      <c r="LY2" s="122"/>
+      <c r="LZ2" s="122"/>
+      <c r="MA2" s="122"/>
+      <c r="MB2" s="122"/>
+      <c r="MC2" s="122"/>
+      <c r="MD2" s="122"/>
+      <c r="ME2" s="122"/>
+      <c r="MF2" s="122"/>
+      <c r="MG2" s="122"/>
+      <c r="MH2" s="122"/>
+      <c r="MI2" s="122"/>
+      <c r="MJ2" s="122"/>
+      <c r="MK2" s="122"/>
+      <c r="ML2" s="122"/>
+      <c r="MM2" s="122"/>
+      <c r="MN2" s="122"/>
+      <c r="MO2" s="122"/>
+      <c r="MP2" s="123"/>
+      <c r="MQ2" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="MR2" s="124"/>
-      <c r="MS2" s="124"/>
-      <c r="MT2" s="124"/>
-      <c r="MU2" s="124"/>
-      <c r="MV2" s="124"/>
-      <c r="MW2" s="124"/>
-      <c r="MX2" s="124"/>
-      <c r="MY2" s="124"/>
-      <c r="MZ2" s="124"/>
-      <c r="NA2" s="124"/>
-      <c r="NB2" s="124"/>
-      <c r="NC2" s="124"/>
-      <c r="ND2" s="124"/>
-      <c r="NE2" s="124"/>
-      <c r="NF2" s="124"/>
-      <c r="NG2" s="124"/>
-      <c r="NH2" s="124"/>
-      <c r="NI2" s="124"/>
-      <c r="NJ2" s="124"/>
-      <c r="NK2" s="124"/>
-      <c r="NL2" s="124"/>
-      <c r="NM2" s="124"/>
-      <c r="NN2" s="124"/>
-      <c r="NO2" s="124"/>
-      <c r="NP2" s="124"/>
-      <c r="NQ2" s="125"/>
-      <c r="NR2" s="123" t="s">
+      <c r="MR2" s="122"/>
+      <c r="MS2" s="122"/>
+      <c r="MT2" s="122"/>
+      <c r="MU2" s="122"/>
+      <c r="MV2" s="122"/>
+      <c r="MW2" s="122"/>
+      <c r="MX2" s="122"/>
+      <c r="MY2" s="122"/>
+      <c r="MZ2" s="122"/>
+      <c r="NA2" s="122"/>
+      <c r="NB2" s="122"/>
+      <c r="NC2" s="122"/>
+      <c r="ND2" s="122"/>
+      <c r="NE2" s="122"/>
+      <c r="NF2" s="122"/>
+      <c r="NG2" s="122"/>
+      <c r="NH2" s="122"/>
+      <c r="NI2" s="122"/>
+      <c r="NJ2" s="122"/>
+      <c r="NK2" s="122"/>
+      <c r="NL2" s="122"/>
+      <c r="NM2" s="122"/>
+      <c r="NN2" s="122"/>
+      <c r="NO2" s="122"/>
+      <c r="NP2" s="122"/>
+      <c r="NQ2" s="123"/>
+      <c r="NR2" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="NS2" s="124"/>
-      <c r="NT2" s="124"/>
-      <c r="NU2" s="124"/>
-      <c r="NV2" s="124"/>
-      <c r="NW2" s="124"/>
-      <c r="NX2" s="124"/>
-      <c r="NY2" s="124"/>
-      <c r="NZ2" s="124"/>
-      <c r="OA2" s="124"/>
-      <c r="OB2" s="124"/>
-      <c r="OC2" s="124"/>
-      <c r="OD2" s="124"/>
-      <c r="OE2" s="124"/>
-      <c r="OF2" s="124"/>
-      <c r="OG2" s="124"/>
-      <c r="OH2" s="124"/>
-      <c r="OI2" s="124"/>
-      <c r="OJ2" s="124"/>
-      <c r="OK2" s="124"/>
-      <c r="OL2" s="124"/>
-      <c r="OM2" s="124"/>
-      <c r="ON2" s="124"/>
-      <c r="OO2" s="124"/>
-      <c r="OP2" s="124"/>
-      <c r="OQ2" s="124"/>
-      <c r="OR2" s="125"/>
-      <c r="OS2" s="123" t="s">
+      <c r="NS2" s="122"/>
+      <c r="NT2" s="122"/>
+      <c r="NU2" s="122"/>
+      <c r="NV2" s="122"/>
+      <c r="NW2" s="122"/>
+      <c r="NX2" s="122"/>
+      <c r="NY2" s="122"/>
+      <c r="NZ2" s="122"/>
+      <c r="OA2" s="122"/>
+      <c r="OB2" s="122"/>
+      <c r="OC2" s="122"/>
+      <c r="OD2" s="122"/>
+      <c r="OE2" s="122"/>
+      <c r="OF2" s="122"/>
+      <c r="OG2" s="122"/>
+      <c r="OH2" s="122"/>
+      <c r="OI2" s="122"/>
+      <c r="OJ2" s="122"/>
+      <c r="OK2" s="122"/>
+      <c r="OL2" s="122"/>
+      <c r="OM2" s="122"/>
+      <c r="ON2" s="122"/>
+      <c r="OO2" s="122"/>
+      <c r="OP2" s="122"/>
+      <c r="OQ2" s="122"/>
+      <c r="OR2" s="123"/>
+      <c r="OS2" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="OT2" s="124"/>
-      <c r="OU2" s="124"/>
-      <c r="OV2" s="124"/>
-      <c r="OW2" s="124"/>
-      <c r="OX2" s="124"/>
-      <c r="OY2" s="124"/>
-      <c r="OZ2" s="124"/>
-      <c r="PA2" s="124"/>
-      <c r="PB2" s="124"/>
-      <c r="PC2" s="124"/>
-      <c r="PD2" s="124"/>
-      <c r="PE2" s="124"/>
-      <c r="PF2" s="124"/>
-      <c r="PG2" s="124"/>
-      <c r="PH2" s="124"/>
-      <c r="PI2" s="124"/>
-      <c r="PJ2" s="124"/>
-      <c r="PK2" s="124"/>
-      <c r="PL2" s="124"/>
-      <c r="PM2" s="124"/>
-      <c r="PN2" s="124"/>
-      <c r="PO2" s="124"/>
-      <c r="PP2" s="124"/>
-      <c r="PQ2" s="124"/>
-      <c r="PR2" s="124"/>
-      <c r="PS2" s="125"/>
+      <c r="OT2" s="122"/>
+      <c r="OU2" s="122"/>
+      <c r="OV2" s="122"/>
+      <c r="OW2" s="122"/>
+      <c r="OX2" s="122"/>
+      <c r="OY2" s="122"/>
+      <c r="OZ2" s="122"/>
+      <c r="PA2" s="122"/>
+      <c r="PB2" s="122"/>
+      <c r="PC2" s="122"/>
+      <c r="PD2" s="122"/>
+      <c r="PE2" s="122"/>
+      <c r="PF2" s="122"/>
+      <c r="PG2" s="122"/>
+      <c r="PH2" s="122"/>
+      <c r="PI2" s="122"/>
+      <c r="PJ2" s="122"/>
+      <c r="PK2" s="122"/>
+      <c r="PL2" s="122"/>
+      <c r="PM2" s="122"/>
+      <c r="PN2" s="122"/>
+      <c r="PO2" s="122"/>
+      <c r="PP2" s="122"/>
+      <c r="PQ2" s="122"/>
+      <c r="PR2" s="122"/>
+      <c r="PS2" s="123"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
@@ -5270,7 +5306,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="122"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5708,7 +5744,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="121" t="str">
+      <c r="B7" s="124" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -6149,7 +6185,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="122"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6587,7 +6623,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="121" t="str">
+      <c r="B9" s="124" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -7028,7 +7064,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="122"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7466,7 +7502,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="121" t="str">
+      <c r="B11" s="124" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7907,7 +7943,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="122"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8345,7 +8381,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="121" t="str">
+      <c r="B13" s="124" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8786,7 +8822,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="122"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -9224,7 +9260,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="121" t="str">
+      <c r="B15" s="124" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9666,7 +9702,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="122"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -10104,7 +10140,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="121" t="str">
+      <c r="B17" s="124" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10545,7 +10581,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="122"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -10983,7 +11019,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="121" t="str">
+      <c r="B19" s="124" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11424,7 +11460,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="122"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11862,7 +11898,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="121" t="str">
+      <c r="B21" s="124" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12303,7 +12339,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="122"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12741,7 +12777,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="121" t="str">
+      <c r="B23" s="124" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -13182,7 +13218,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="122"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13620,7 +13656,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="121" t="str">
+      <c r="B25" s="124" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -14061,7 +14097,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="122"/>
+      <c r="B26" s="125"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14499,7 +14535,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="121" t="str">
+      <c r="B27" s="124" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -14940,7 +14976,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="122"/>
+      <c r="B28" s="125"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15378,7 +15414,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="121" t="str">
+      <c r="B29" s="124" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15819,7 +15855,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="122"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16257,7 +16293,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="121" t="str">
+      <c r="B31" s="124" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16698,7 +16734,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="122"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -18020,13 +18056,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="OS2:PS2"/>
-    <mergeCell ref="IM2:JM2"/>
-    <mergeCell ref="JN2:KN2"/>
-    <mergeCell ref="KO2:LO2"/>
-    <mergeCell ref="LP2:MP2"/>
-    <mergeCell ref="MQ2:NQ2"/>
-    <mergeCell ref="NR2:OR2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="HL2:IL2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="CG2:DG2"/>
+    <mergeCell ref="DH2:EH2"/>
+    <mergeCell ref="EI2:FI2"/>
+    <mergeCell ref="FJ2:GJ2"/>
+    <mergeCell ref="GK2:HK2"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="D2:AD2"/>
@@ -18043,14 +18080,13 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="HL2:IL2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="CG2:DG2"/>
-    <mergeCell ref="DH2:EH2"/>
-    <mergeCell ref="EI2:FI2"/>
-    <mergeCell ref="FJ2:GJ2"/>
-    <mergeCell ref="GK2:HK2"/>
+    <mergeCell ref="OS2:PS2"/>
+    <mergeCell ref="IM2:JM2"/>
+    <mergeCell ref="JN2:KN2"/>
+    <mergeCell ref="KO2:LO2"/>
+    <mergeCell ref="LP2:MP2"/>
+    <mergeCell ref="MQ2:NQ2"/>
+    <mergeCell ref="NR2:OR2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C33">
@@ -20717,10 +20753,10 @@
   <sheetPr codeName="Feuil9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I307"/>
+  <dimension ref="A1:I310"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A123" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A138" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22079,7 +22115,9 @@
       <c r="B131" s="79">
         <v>3</v>
       </c>
-      <c r="C131" s="80"/>
+      <c r="C131" s="80" t="s">
+        <v>106</v>
+      </c>
       <c r="D131" s="80"/>
     </row>
     <row r="132" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -22142,165 +22180,249 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A138" s="9"/>
-      <c r="B138" s="8"/>
+      <c r="A138" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B138" s="8">
+        <v>1</v>
+      </c>
       <c r="C138" s="13"/>
       <c r="D138" s="13"/>
     </row>
-    <row r="139" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A139" s="5"/>
-      <c r="B139" s="6"/>
-      <c r="C139" s="14"/>
+    <row r="139" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B139" s="6">
+        <v>2</v>
+      </c>
+      <c r="C139" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D139" s="14"/>
     </row>
-    <row r="140" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A140" s="5"/>
-      <c r="B140" s="6"/>
-      <c r="C140" s="14"/>
-      <c r="D140" s="14"/>
-    </row>
-    <row r="141" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A141" s="5"/>
-      <c r="B141" s="6"/>
-      <c r="C141" s="14"/>
-      <c r="D141" s="14"/>
-    </row>
-    <row r="142" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A142" s="5"/>
-      <c r="B142" s="6"/>
-      <c r="C142" s="14"/>
-      <c r="D142" s="14"/>
-    </row>
-    <row r="143" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A143" s="5"/>
-      <c r="B143" s="6"/>
-      <c r="C143" s="14"/>
-      <c r="D143" s="14"/>
+    <row r="140" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B140" s="6">
+        <v>5</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D140" s="108" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B141" s="6">
+        <v>1</v>
+      </c>
+      <c r="C141" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D141" s="108" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A142" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B142" s="6">
+        <v>1</v>
+      </c>
+      <c r="C142" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D142" s="108" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A143" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B143" s="6">
+        <v>2</v>
+      </c>
+      <c r="C143" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D143" s="108"/>
     </row>
     <row r="144" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A144" s="5"/>
-      <c r="B144" s="6"/>
-      <c r="C144" s="14"/>
+      <c r="A144" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B144" s="6">
+        <v>3</v>
+      </c>
+      <c r="C144" s="14" t="s">
+        <v>118</v>
+      </c>
       <c r="D144" s="14"/>
     </row>
     <row r="145" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
       <c r="B145" s="6"/>
-      <c r="C145" s="14"/>
+      <c r="C145" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="D145" s="14"/>
     </row>
     <row r="146" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A146" s="5"/>
-      <c r="B146" s="6"/>
-      <c r="C146" s="14"/>
+      <c r="A146" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B146" s="6">
+        <v>4</v>
+      </c>
+      <c r="C146" s="14" t="s">
+        <v>125</v>
+      </c>
       <c r="D146" s="14"/>
     </row>
-    <row r="147" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A147" s="6"/>
-      <c r="B147" s="6"/>
-      <c r="C147" s="14"/>
+    <row r="147" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A147" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B147" s="6">
+        <v>2</v>
+      </c>
+      <c r="C147" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="D147" s="14"/>
     </row>
     <row r="148" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A148" s="6"/>
-      <c r="B148" s="6"/>
-      <c r="C148" s="14"/>
+      <c r="A148" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B148" s="6">
+        <v>1</v>
+      </c>
+      <c r="C148" s="14" t="s">
+        <v>128</v>
+      </c>
       <c r="D148" s="14"/>
     </row>
     <row r="149" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6"/>
-      <c r="C149" s="14"/>
+      <c r="A149" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B149" s="6">
+        <v>1</v>
+      </c>
+      <c r="C149" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="D149" s="14"/>
     </row>
-    <row r="150" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A150" s="79"/>
-      <c r="B150" s="79"/>
-      <c r="C150" s="80"/>
-      <c r="D150" s="80"/>
+    <row r="150" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A150" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B150" s="6">
+        <v>1</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D150" s="14"/>
     </row>
     <row r="151" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A151" s="79"/>
-      <c r="B151" s="79"/>
-      <c r="C151" s="80"/>
-      <c r="D151" s="80"/>
-    </row>
-    <row r="152" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="15"/>
-    </row>
-    <row r="153" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="76" t="s">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+    </row>
+    <row r="152" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A152" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B152" s="6">
+        <v>3</v>
+      </c>
+      <c r="C152" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D152" s="14"/>
+    </row>
+    <row r="153" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A153" s="79"/>
+      <c r="B153" s="79"/>
+      <c r="C153" s="80"/>
+      <c r="D153" s="80"/>
+    </row>
+    <row r="154" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A154" s="79"/>
+      <c r="B154" s="79"/>
+      <c r="C154" s="80"/>
+      <c r="D154" s="80"/>
+    </row>
+    <row r="155" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="7"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="15"/>
+      <c r="D155" s="15"/>
+    </row>
+    <row r="156" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B153" s="76">
-        <f>SUM(B138:B152)</f>
-        <v>0</v>
-      </c>
-      <c r="C153" s="107" t="s">
+      <c r="B156" s="76">
+        <f>SUM(B138:B155)</f>
+        <v>27</v>
+      </c>
+      <c r="C156" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D153" s="77"/>
-    </row>
-    <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="78"/>
-      <c r="B154" s="78"/>
-      <c r="C154" s="78"/>
-      <c r="D154" s="78"/>
-    </row>
-    <row r="155" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="71" t="s">
+      <c r="D156" s="77"/>
+    </row>
+    <row r="157" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="78"/>
+      <c r="B157" s="78"/>
+      <c r="C157" s="78"/>
+      <c r="D157" s="78"/>
+    </row>
+    <row r="158" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B155" s="72">
+      <c r="B158" s="72">
         <v>9</v>
       </c>
-      <c r="C155" s="73" t="s">
+      <c r="C158" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D155" s="82">
+      <c r="D158" s="82">
         <v>42899</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="74" t="s">
+    <row r="159" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B156" s="75" t="s">
+      <c r="B159" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C156" s="74" t="s">
+      <c r="C159" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D156" s="74" t="s">
+      <c r="D159" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A157" s="9"/>
-      <c r="B157" s="8"/>
-      <c r="C157" s="13"/>
-      <c r="D157" s="13"/>
-    </row>
-    <row r="158" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="5"/>
-      <c r="B158" s="6"/>
-      <c r="C158" s="14"/>
-      <c r="D158" s="14"/>
-    </row>
-    <row r="159" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A159" s="5"/>
-      <c r="B159" s="6"/>
-      <c r="C159" s="14"/>
-      <c r="D159" s="14"/>
-    </row>
     <row r="160" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A160" s="5"/>
-      <c r="B160" s="6"/>
-      <c r="C160" s="14"/>
-      <c r="D160" s="14"/>
+      <c r="A160" s="9"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
     </row>
     <row r="161" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A161" s="5"/>
@@ -22333,115 +22455,123 @@
       <c r="D165" s="14"/>
     </row>
     <row r="166" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A166" s="6"/>
+      <c r="A166" s="5"/>
       <c r="B166" s="6"/>
       <c r="C166" s="14"/>
       <c r="D166" s="14"/>
     </row>
     <row r="167" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A167" s="6"/>
+      <c r="A167" s="5"/>
       <c r="B167" s="6"/>
       <c r="C167" s="14"/>
       <c r="D167" s="14"/>
     </row>
     <row r="168" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="6"/>
+      <c r="A168" s="5"/>
       <c r="B168" s="6"/>
       <c r="C168" s="14"/>
       <c r="D168" s="14"/>
     </row>
     <row r="169" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A169" s="79"/>
-      <c r="B169" s="79"/>
-      <c r="C169" s="80"/>
-      <c r="D169" s="80"/>
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="14"/>
+      <c r="D169" s="14"/>
     </row>
     <row r="170" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A170" s="79"/>
-      <c r="B170" s="79"/>
-      <c r="C170" s="80"/>
-      <c r="D170" s="80"/>
-    </row>
-    <row r="171" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="7"/>
-      <c r="B171" s="7"/>
-      <c r="C171" s="15"/>
-      <c r="D171" s="15"/>
-    </row>
-    <row r="172" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="76" t="s">
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="14"/>
+      <c r="D170" s="14"/>
+    </row>
+    <row r="171" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="14"/>
+      <c r="D171" s="14"/>
+    </row>
+    <row r="172" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A172" s="79"/>
+      <c r="B172" s="79"/>
+      <c r="C172" s="80"/>
+      <c r="D172" s="80"/>
+    </row>
+    <row r="173" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A173" s="79"/>
+      <c r="B173" s="79"/>
+      <c r="C173" s="80"/>
+      <c r="D173" s="80"/>
+    </row>
+    <row r="174" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="7"/>
+      <c r="B174" s="7"/>
+      <c r="C174" s="15"/>
+      <c r="D174" s="15"/>
+    </row>
+    <row r="175" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B172" s="76">
-        <f>SUM(B157:B171)</f>
+      <c r="B175" s="76">
+        <f>SUM(B160:B174)</f>
         <v>0</v>
       </c>
-      <c r="C172" s="107" t="s">
+      <c r="C175" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D172" s="77"/>
-    </row>
-    <row r="173" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="78"/>
-      <c r="B173" s="78"/>
-      <c r="C173" s="78"/>
-      <c r="D173" s="78"/>
-    </row>
-    <row r="174" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="71" t="s">
+      <c r="D175" s="77"/>
+    </row>
+    <row r="176" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="78"/>
+      <c r="B176" s="78"/>
+      <c r="C176" s="78"/>
+      <c r="D176" s="78"/>
+    </row>
+    <row r="177" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B174" s="72">
+      <c r="B177" s="72">
         <v>10</v>
       </c>
-      <c r="C174" s="73" t="s">
+      <c r="C177" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D174" s="82">
+      <c r="D177" s="82">
         <v>42900</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="74" t="s">
+    <row r="178" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B175" s="75" t="s">
+      <c r="B178" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C175" s="74" t="s">
+      <c r="C178" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D175" s="74" t="s">
+      <c r="D178" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A176" s="9"/>
-      <c r="B176" s="8"/>
-      <c r="C176" s="13"/>
-      <c r="D176" s="13"/>
-    </row>
-    <row r="177" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A177" s="5"/>
-      <c r="B177" s="6"/>
-      <c r="C177" s="14"/>
-      <c r="D177" s="14"/>
-    </row>
-    <row r="178" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A178" s="5"/>
-      <c r="B178" s="6"/>
-      <c r="C178" s="14"/>
-      <c r="D178" s="14"/>
-    </row>
     <row r="179" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A179" s="5"/>
-      <c r="B179" s="6"/>
-      <c r="C179" s="14"/>
-      <c r="D179" s="14"/>
+      <c r="A179" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B179" s="8">
+        <v>1</v>
+      </c>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
     </row>
     <row r="180" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A180" s="5"/>
-      <c r="B180" s="6"/>
+      <c r="A180" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B180" s="6">
+        <v>2</v>
+      </c>
       <c r="C180" s="14"/>
       <c r="D180" s="14"/>
     </row>
@@ -22470,111 +22600,111 @@
       <c r="D184" s="14"/>
     </row>
     <row r="185" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A185" s="6"/>
+      <c r="A185" s="5"/>
       <c r="B185" s="6"/>
       <c r="C185" s="14"/>
       <c r="D185" s="14"/>
     </row>
     <row r="186" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A186" s="6"/>
+      <c r="A186" s="5"/>
       <c r="B186" s="6"/>
       <c r="C186" s="14"/>
       <c r="D186" s="14"/>
     </row>
     <row r="187" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A187" s="6"/>
+      <c r="A187" s="5"/>
       <c r="B187" s="6"/>
       <c r="C187" s="14"/>
       <c r="D187" s="14"/>
     </row>
     <row r="188" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A188" s="79"/>
-      <c r="B188" s="79"/>
-      <c r="C188" s="80"/>
-      <c r="D188" s="80"/>
+      <c r="A188" s="6"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="14"/>
+      <c r="D188" s="14"/>
     </row>
     <row r="189" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A189" s="79"/>
-      <c r="B189" s="79"/>
-      <c r="C189" s="80"/>
-      <c r="D189" s="80"/>
-    </row>
-    <row r="190" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="7"/>
-      <c r="B190" s="7"/>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15"/>
-    </row>
-    <row r="191" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="76" t="s">
+      <c r="A189" s="6"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="14"/>
+      <c r="D189" s="14"/>
+    </row>
+    <row r="190" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="14"/>
+      <c r="D190" s="14"/>
+    </row>
+    <row r="191" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A191" s="79"/>
+      <c r="B191" s="79"/>
+      <c r="C191" s="80"/>
+      <c r="D191" s="80"/>
+    </row>
+    <row r="192" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A192" s="79"/>
+      <c r="B192" s="79"/>
+      <c r="C192" s="80"/>
+      <c r="D192" s="80"/>
+    </row>
+    <row r="193" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="7"/>
+      <c r="B193" s="7"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="15"/>
+    </row>
+    <row r="194" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B191" s="76">
-        <f>SUM(B176:B190)</f>
-        <v>0</v>
-      </c>
-      <c r="C191" s="107" t="s">
+      <c r="B194" s="76">
+        <f>SUM(B179:B193)</f>
+        <v>3</v>
+      </c>
+      <c r="C194" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="77"/>
-    </row>
-    <row r="192" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="78"/>
-      <c r="B192" s="78"/>
-      <c r="C192" s="78"/>
-      <c r="D192" s="78"/>
-    </row>
-    <row r="193" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="71" t="s">
+      <c r="D194" s="77"/>
+    </row>
+    <row r="195" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="78"/>
+      <c r="B195" s="78"/>
+      <c r="C195" s="78"/>
+      <c r="D195" s="78"/>
+    </row>
+    <row r="196" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B193" s="72">
+      <c r="B196" s="72">
         <v>11</v>
       </c>
-      <c r="C193" s="73" t="s">
+      <c r="C196" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D193" s="82">
+      <c r="D196" s="82">
         <v>42902</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="74" t="s">
+    <row r="197" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B194" s="75" t="s">
+      <c r="B197" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C194" s="74" t="s">
+      <c r="C197" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D194" s="74" t="s">
+      <c r="D197" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A195" s="9"/>
-      <c r="B195" s="8"/>
-      <c r="C195" s="13"/>
-      <c r="D195" s="13"/>
-    </row>
-    <row r="196" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A196" s="5"/>
-      <c r="B196" s="6"/>
-      <c r="C196" s="14"/>
-      <c r="D196" s="14"/>
-    </row>
-    <row r="197" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A197" s="5"/>
-      <c r="B197" s="6"/>
-      <c r="C197" s="14"/>
-      <c r="D197" s="14"/>
-    </row>
     <row r="198" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A198" s="5"/>
-      <c r="B198" s="6"/>
-      <c r="C198" s="14"/>
-      <c r="D198" s="14"/>
+      <c r="A198" s="9"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="13"/>
+      <c r="D198" s="13"/>
     </row>
     <row r="199" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A199" s="5"/>
@@ -22607,111 +22737,111 @@
       <c r="D203" s="14"/>
     </row>
     <row r="204" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A204" s="6"/>
+      <c r="A204" s="5"/>
       <c r="B204" s="6"/>
       <c r="C204" s="14"/>
       <c r="D204" s="14"/>
     </row>
     <row r="205" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A205" s="6"/>
+      <c r="A205" s="5"/>
       <c r="B205" s="6"/>
       <c r="C205" s="14"/>
       <c r="D205" s="14"/>
     </row>
     <row r="206" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A206" s="6"/>
+      <c r="A206" s="5"/>
       <c r="B206" s="6"/>
       <c r="C206" s="14"/>
       <c r="D206" s="14"/>
     </row>
     <row r="207" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A207" s="79"/>
-      <c r="B207" s="79"/>
-      <c r="C207" s="80"/>
-      <c r="D207" s="80"/>
+      <c r="A207" s="6"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="14"/>
+      <c r="D207" s="14"/>
     </row>
     <row r="208" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A208" s="79"/>
-      <c r="B208" s="79"/>
-      <c r="C208" s="80"/>
-      <c r="D208" s="80"/>
-    </row>
-    <row r="209" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="7"/>
-      <c r="B209" s="7"/>
-      <c r="C209" s="15"/>
-      <c r="D209" s="15"/>
-    </row>
-    <row r="210" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="76" t="s">
+      <c r="A208" s="6"/>
+      <c r="B208" s="6"/>
+      <c r="C208" s="14"/>
+      <c r="D208" s="14"/>
+    </row>
+    <row r="209" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A209" s="6"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="14"/>
+      <c r="D209" s="14"/>
+    </row>
+    <row r="210" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A210" s="79"/>
+      <c r="B210" s="79"/>
+      <c r="C210" s="80"/>
+      <c r="D210" s="80"/>
+    </row>
+    <row r="211" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A211" s="79"/>
+      <c r="B211" s="79"/>
+      <c r="C211" s="80"/>
+      <c r="D211" s="80"/>
+    </row>
+    <row r="212" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="7"/>
+      <c r="B212" s="7"/>
+      <c r="C212" s="15"/>
+      <c r="D212" s="15"/>
+    </row>
+    <row r="213" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B210" s="76">
-        <f>SUM(B195:B209)</f>
+      <c r="B213" s="76">
+        <f>SUM(B198:B212)</f>
         <v>0</v>
       </c>
-      <c r="C210" s="107" t="s">
+      <c r="C213" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D210" s="77"/>
-    </row>
-    <row r="211" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A211" s="78"/>
-      <c r="B211" s="78"/>
-      <c r="C211" s="78"/>
-      <c r="D211" s="78"/>
-    </row>
-    <row r="212" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="71" t="s">
+      <c r="D213" s="77"/>
+    </row>
+    <row r="214" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A214" s="78"/>
+      <c r="B214" s="78"/>
+      <c r="C214" s="78"/>
+      <c r="D214" s="78"/>
+    </row>
+    <row r="215" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B212" s="72">
+      <c r="B215" s="72">
         <v>12</v>
       </c>
-      <c r="C212" s="73" t="s">
+      <c r="C215" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D212" s="82">
+      <c r="D215" s="82">
         <v>42912</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="74" t="s">
+    <row r="216" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B213" s="75" t="s">
+      <c r="B216" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C213" s="74" t="s">
+      <c r="C216" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D213" s="74" t="s">
+      <c r="D216" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A214" s="9"/>
-      <c r="B214" s="8"/>
-      <c r="C214" s="13"/>
-      <c r="D214" s="13"/>
-    </row>
-    <row r="215" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A215" s="5"/>
-      <c r="B215" s="6"/>
-      <c r="C215" s="14"/>
-      <c r="D215" s="14"/>
-    </row>
-    <row r="216" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A216" s="5"/>
-      <c r="B216" s="6"/>
-      <c r="C216" s="14"/>
-      <c r="D216" s="14"/>
-    </row>
     <row r="217" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A217" s="5"/>
-      <c r="B217" s="6"/>
-      <c r="C217" s="14"/>
-      <c r="D217" s="14"/>
+      <c r="A217" s="9"/>
+      <c r="B217" s="8"/>
+      <c r="C217" s="13"/>
+      <c r="D217" s="13"/>
     </row>
     <row r="218" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A218" s="5"/>
@@ -22744,111 +22874,111 @@
       <c r="D222" s="14"/>
     </row>
     <row r="223" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A223" s="6"/>
+      <c r="A223" s="5"/>
       <c r="B223" s="6"/>
       <c r="C223" s="14"/>
       <c r="D223" s="14"/>
     </row>
     <row r="224" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A224" s="6"/>
+      <c r="A224" s="5"/>
       <c r="B224" s="6"/>
       <c r="C224" s="14"/>
       <c r="D224" s="14"/>
     </row>
     <row r="225" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A225" s="6"/>
+      <c r="A225" s="5"/>
       <c r="B225" s="6"/>
       <c r="C225" s="14"/>
       <c r="D225" s="14"/>
     </row>
     <row r="226" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A226" s="79"/>
-      <c r="B226" s="79"/>
-      <c r="C226" s="80"/>
-      <c r="D226" s="80"/>
+      <c r="A226" s="6"/>
+      <c r="B226" s="6"/>
+      <c r="C226" s="14"/>
+      <c r="D226" s="14"/>
     </row>
     <row r="227" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A227" s="79"/>
-      <c r="B227" s="79"/>
-      <c r="C227" s="80"/>
-      <c r="D227" s="80"/>
-    </row>
-    <row r="228" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="7"/>
-      <c r="B228" s="7"/>
-      <c r="C228" s="15"/>
-      <c r="D228" s="15"/>
-    </row>
-    <row r="229" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="76" t="s">
+      <c r="A227" s="6"/>
+      <c r="B227" s="6"/>
+      <c r="C227" s="14"/>
+      <c r="D227" s="14"/>
+    </row>
+    <row r="228" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A228" s="6"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="14"/>
+      <c r="D228" s="14"/>
+    </row>
+    <row r="229" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A229" s="79"/>
+      <c r="B229" s="79"/>
+      <c r="C229" s="80"/>
+      <c r="D229" s="80"/>
+    </row>
+    <row r="230" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A230" s="79"/>
+      <c r="B230" s="79"/>
+      <c r="C230" s="80"/>
+      <c r="D230" s="80"/>
+    </row>
+    <row r="231" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="7"/>
+      <c r="B231" s="7"/>
+      <c r="C231" s="15"/>
+      <c r="D231" s="15"/>
+    </row>
+    <row r="232" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B229" s="76">
-        <f>SUM(B214:B228)</f>
+      <c r="B232" s="76">
+        <f>SUM(B217:B231)</f>
         <v>0</v>
       </c>
-      <c r="C229" s="107" t="s">
+      <c r="C232" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D229" s="77"/>
-    </row>
-    <row r="230" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A230" s="78"/>
-      <c r="B230" s="78"/>
-      <c r="C230" s="78"/>
-      <c r="D230" s="78"/>
-    </row>
-    <row r="231" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="71" t="s">
+      <c r="D232" s="77"/>
+    </row>
+    <row r="233" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="78"/>
+      <c r="B233" s="78"/>
+      <c r="C233" s="78"/>
+      <c r="D233" s="78"/>
+    </row>
+    <row r="234" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B231" s="72">
+      <c r="B234" s="72">
         <v>13</v>
       </c>
-      <c r="C231" s="73" t="s">
+      <c r="C234" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D231" s="82">
+      <c r="D234" s="82">
         <v>42968</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="74" t="s">
+    <row r="235" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B232" s="75" t="s">
+      <c r="B235" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C232" s="74" t="s">
+      <c r="C235" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D232" s="74" t="s">
+      <c r="D235" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A233" s="9"/>
-      <c r="B233" s="8"/>
-      <c r="C233" s="13"/>
-      <c r="D233" s="13"/>
-    </row>
-    <row r="234" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A234" s="5"/>
-      <c r="B234" s="6"/>
-      <c r="C234" s="14"/>
-      <c r="D234" s="14"/>
-    </row>
-    <row r="235" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A235" s="5"/>
-      <c r="B235" s="6"/>
-      <c r="C235" s="14"/>
-      <c r="D235" s="14"/>
-    </row>
     <row r="236" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A236" s="5"/>
-      <c r="B236" s="6"/>
-      <c r="C236" s="14"/>
-      <c r="D236" s="14"/>
+      <c r="A236" s="9"/>
+      <c r="B236" s="8"/>
+      <c r="C236" s="13"/>
+      <c r="D236" s="13"/>
     </row>
     <row r="237" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A237" s="5"/>
@@ -22881,111 +23011,111 @@
       <c r="D241" s="14"/>
     </row>
     <row r="242" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A242" s="6"/>
+      <c r="A242" s="5"/>
       <c r="B242" s="6"/>
       <c r="C242" s="14"/>
       <c r="D242" s="14"/>
     </row>
     <row r="243" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A243" s="6"/>
+      <c r="A243" s="5"/>
       <c r="B243" s="6"/>
       <c r="C243" s="14"/>
       <c r="D243" s="14"/>
     </row>
     <row r="244" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A244" s="6"/>
+      <c r="A244" s="5"/>
       <c r="B244" s="6"/>
       <c r="C244" s="14"/>
       <c r="D244" s="14"/>
     </row>
     <row r="245" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A245" s="79"/>
-      <c r="B245" s="79"/>
-      <c r="C245" s="80"/>
-      <c r="D245" s="80"/>
+      <c r="A245" s="6"/>
+      <c r="B245" s="6"/>
+      <c r="C245" s="14"/>
+      <c r="D245" s="14"/>
     </row>
     <row r="246" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A246" s="79"/>
-      <c r="B246" s="79"/>
-      <c r="C246" s="80"/>
-      <c r="D246" s="80"/>
-    </row>
-    <row r="247" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="7"/>
-      <c r="B247" s="7"/>
-      <c r="C247" s="15"/>
-      <c r="D247" s="15"/>
-    </row>
-    <row r="248" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="76" t="s">
+      <c r="A246" s="6"/>
+      <c r="B246" s="6"/>
+      <c r="C246" s="14"/>
+      <c r="D246" s="14"/>
+    </row>
+    <row r="247" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A247" s="6"/>
+      <c r="B247" s="6"/>
+      <c r="C247" s="14"/>
+      <c r="D247" s="14"/>
+    </row>
+    <row r="248" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A248" s="79"/>
+      <c r="B248" s="79"/>
+      <c r="C248" s="80"/>
+      <c r="D248" s="80"/>
+    </row>
+    <row r="249" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A249" s="79"/>
+      <c r="B249" s="79"/>
+      <c r="C249" s="80"/>
+      <c r="D249" s="80"/>
+    </row>
+    <row r="250" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="7"/>
+      <c r="B250" s="7"/>
+      <c r="C250" s="15"/>
+      <c r="D250" s="15"/>
+    </row>
+    <row r="251" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B248" s="76">
-        <f>SUM(B233:B247)</f>
+      <c r="B251" s="76">
+        <f>SUM(B236:B250)</f>
         <v>0</v>
       </c>
-      <c r="C248" s="107" t="s">
+      <c r="C251" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D248" s="77"/>
-    </row>
-    <row r="249" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="78"/>
-      <c r="B249" s="78"/>
-      <c r="C249" s="78"/>
-      <c r="D249" s="78"/>
-    </row>
-    <row r="250" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="71" t="s">
+      <c r="D251" s="77"/>
+    </row>
+    <row r="252" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A252" s="78"/>
+      <c r="B252" s="78"/>
+      <c r="C252" s="78"/>
+      <c r="D252" s="78"/>
+    </row>
+    <row r="253" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B250" s="72">
+      <c r="B253" s="72">
         <v>14</v>
       </c>
-      <c r="C250" s="73" t="s">
+      <c r="C253" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D250" s="82">
+      <c r="D253" s="82">
         <v>42975</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="74" t="s">
+    <row r="254" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B251" s="75" t="s">
+      <c r="B254" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C251" s="74" t="s">
+      <c r="C254" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D251" s="74" t="s">
+      <c r="D254" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A252" s="9"/>
-      <c r="B252" s="8"/>
-      <c r="C252" s="13"/>
-      <c r="D252" s="13"/>
-    </row>
-    <row r="253" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A253" s="5"/>
-      <c r="B253" s="6"/>
-      <c r="C253" s="14"/>
-      <c r="D253" s="14"/>
-    </row>
-    <row r="254" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A254" s="5"/>
-      <c r="B254" s="6"/>
-      <c r="C254" s="14"/>
-      <c r="D254" s="14"/>
-    </row>
     <row r="255" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A255" s="5"/>
-      <c r="B255" s="6"/>
-      <c r="C255" s="14"/>
-      <c r="D255" s="14"/>
+      <c r="A255" s="9"/>
+      <c r="B255" s="8"/>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
     </row>
     <row r="256" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A256" s="5"/>
@@ -23018,111 +23148,111 @@
       <c r="D260" s="14"/>
     </row>
     <row r="261" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A261" s="6"/>
+      <c r="A261" s="5"/>
       <c r="B261" s="6"/>
       <c r="C261" s="14"/>
       <c r="D261" s="14"/>
     </row>
     <row r="262" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A262" s="6"/>
+      <c r="A262" s="5"/>
       <c r="B262" s="6"/>
       <c r="C262" s="14"/>
       <c r="D262" s="14"/>
     </row>
     <row r="263" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A263" s="6"/>
+      <c r="A263" s="5"/>
       <c r="B263" s="6"/>
       <c r="C263" s="14"/>
       <c r="D263" s="14"/>
     </row>
     <row r="264" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A264" s="79"/>
-      <c r="B264" s="79"/>
-      <c r="C264" s="80"/>
-      <c r="D264" s="80"/>
+      <c r="A264" s="6"/>
+      <c r="B264" s="6"/>
+      <c r="C264" s="14"/>
+      <c r="D264" s="14"/>
     </row>
     <row r="265" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A265" s="79"/>
-      <c r="B265" s="79"/>
-      <c r="C265" s="80"/>
-      <c r="D265" s="80"/>
-    </row>
-    <row r="266" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="7"/>
-      <c r="B266" s="7"/>
-      <c r="C266" s="15"/>
-      <c r="D266" s="15"/>
-    </row>
-    <row r="267" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="76" t="s">
+      <c r="A265" s="6"/>
+      <c r="B265" s="6"/>
+      <c r="C265" s="14"/>
+      <c r="D265" s="14"/>
+    </row>
+    <row r="266" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A266" s="6"/>
+      <c r="B266" s="6"/>
+      <c r="C266" s="14"/>
+      <c r="D266" s="14"/>
+    </row>
+    <row r="267" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A267" s="79"/>
+      <c r="B267" s="79"/>
+      <c r="C267" s="80"/>
+      <c r="D267" s="80"/>
+    </row>
+    <row r="268" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A268" s="79"/>
+      <c r="B268" s="79"/>
+      <c r="C268" s="80"/>
+      <c r="D268" s="80"/>
+    </row>
+    <row r="269" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="7"/>
+      <c r="B269" s="7"/>
+      <c r="C269" s="15"/>
+      <c r="D269" s="15"/>
+    </row>
+    <row r="270" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B267" s="76">
-        <f>SUM(B252:B266)</f>
+      <c r="B270" s="76">
+        <f>SUM(B255:B269)</f>
         <v>0</v>
       </c>
-      <c r="C267" s="107" t="s">
+      <c r="C270" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D267" s="77"/>
-    </row>
-    <row r="268" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A268" s="78"/>
-      <c r="B268" s="78"/>
-      <c r="C268" s="78"/>
-      <c r="D268" s="78"/>
-    </row>
-    <row r="269" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="71" t="s">
+      <c r="D270" s="77"/>
+    </row>
+    <row r="271" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A271" s="78"/>
+      <c r="B271" s="78"/>
+      <c r="C271" s="78"/>
+      <c r="D271" s="78"/>
+    </row>
+    <row r="272" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B269" s="72">
+      <c r="B272" s="72">
         <v>15</v>
       </c>
-      <c r="C269" s="73" t="s">
+      <c r="C272" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D269" s="82">
+      <c r="D272" s="82">
         <v>42982</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="74" t="s">
+    <row r="273" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B270" s="75" t="s">
+      <c r="B273" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C270" s="74" t="s">
+      <c r="C273" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D270" s="74" t="s">
+      <c r="D273" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A271" s="9"/>
-      <c r="B271" s="8"/>
-      <c r="C271" s="13"/>
-      <c r="D271" s="13"/>
-    </row>
-    <row r="272" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A272" s="5"/>
-      <c r="B272" s="6"/>
-      <c r="C272" s="14"/>
-      <c r="D272" s="14"/>
-    </row>
-    <row r="273" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A273" s="5"/>
-      <c r="B273" s="6"/>
-      <c r="C273" s="14"/>
-      <c r="D273" s="14"/>
-    </row>
     <row r="274" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A274" s="5"/>
-      <c r="B274" s="6"/>
-      <c r="C274" s="14"/>
-      <c r="D274" s="14"/>
+      <c r="A274" s="9"/>
+      <c r="B274" s="8"/>
+      <c r="C274" s="13"/>
+      <c r="D274" s="13"/>
     </row>
     <row r="275" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A275" s="5"/>
@@ -23155,111 +23285,111 @@
       <c r="D279" s="14"/>
     </row>
     <row r="280" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A280" s="6"/>
+      <c r="A280" s="5"/>
       <c r="B280" s="6"/>
       <c r="C280" s="14"/>
       <c r="D280" s="14"/>
     </row>
     <row r="281" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A281" s="6"/>
+      <c r="A281" s="5"/>
       <c r="B281" s="6"/>
       <c r="C281" s="14"/>
       <c r="D281" s="14"/>
     </row>
     <row r="282" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A282" s="6"/>
+      <c r="A282" s="5"/>
       <c r="B282" s="6"/>
       <c r="C282" s="14"/>
       <c r="D282" s="14"/>
     </row>
     <row r="283" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A283" s="79"/>
-      <c r="B283" s="79"/>
-      <c r="C283" s="80"/>
-      <c r="D283" s="80"/>
+      <c r="A283" s="6"/>
+      <c r="B283" s="6"/>
+      <c r="C283" s="14"/>
+      <c r="D283" s="14"/>
     </row>
     <row r="284" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A284" s="79"/>
-      <c r="B284" s="79"/>
-      <c r="C284" s="80"/>
-      <c r="D284" s="80"/>
-    </row>
-    <row r="285" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="7"/>
-      <c r="B285" s="7"/>
-      <c r="C285" s="15"/>
-      <c r="D285" s="15"/>
-    </row>
-    <row r="286" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="76" t="s">
+      <c r="A284" s="6"/>
+      <c r="B284" s="6"/>
+      <c r="C284" s="14"/>
+      <c r="D284" s="14"/>
+    </row>
+    <row r="285" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A285" s="6"/>
+      <c r="B285" s="6"/>
+      <c r="C285" s="14"/>
+      <c r="D285" s="14"/>
+    </row>
+    <row r="286" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A286" s="79"/>
+      <c r="B286" s="79"/>
+      <c r="C286" s="80"/>
+      <c r="D286" s="80"/>
+    </row>
+    <row r="287" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A287" s="79"/>
+      <c r="B287" s="79"/>
+      <c r="C287" s="80"/>
+      <c r="D287" s="80"/>
+    </row>
+    <row r="288" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="7"/>
+      <c r="B288" s="7"/>
+      <c r="C288" s="15"/>
+      <c r="D288" s="15"/>
+    </row>
+    <row r="289" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B286" s="76">
-        <f>SUM(B271:B285)</f>
+      <c r="B289" s="76">
+        <f>SUM(B274:B288)</f>
         <v>0</v>
       </c>
-      <c r="C286" s="107" t="s">
+      <c r="C289" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D286" s="77"/>
-    </row>
-    <row r="287" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A287" s="78"/>
-      <c r="B287" s="78"/>
-      <c r="C287" s="78"/>
-      <c r="D287" s="78"/>
-    </row>
-    <row r="288" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="71" t="s">
+      <c r="D289" s="77"/>
+    </row>
+    <row r="290" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A290" s="78"/>
+      <c r="B290" s="78"/>
+      <c r="C290" s="78"/>
+      <c r="D290" s="78"/>
+    </row>
+    <row r="291" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B288" s="72">
+      <c r="B291" s="72">
         <v>16</v>
       </c>
-      <c r="C288" s="73" t="s">
+      <c r="C291" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D288" s="82">
+      <c r="D291" s="82">
         <v>42989</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="74" t="s">
+    <row r="292" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B289" s="75" t="s">
+      <c r="B292" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C289" s="74" t="s">
+      <c r="C292" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D289" s="74" t="s">
+      <c r="D292" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A290" s="9"/>
-      <c r="B290" s="8"/>
-      <c r="C290" s="13"/>
-      <c r="D290" s="13"/>
-    </row>
-    <row r="291" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A291" s="5"/>
-      <c r="B291" s="6"/>
-      <c r="C291" s="14"/>
-      <c r="D291" s="14"/>
-    </row>
-    <row r="292" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A292" s="5"/>
-      <c r="B292" s="6"/>
-      <c r="C292" s="14"/>
-      <c r="D292" s="14"/>
-    </row>
     <row r="293" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A293" s="5"/>
-      <c r="B293" s="6"/>
-      <c r="C293" s="14"/>
-      <c r="D293" s="14"/>
+      <c r="A293" s="9"/>
+      <c r="B293" s="8"/>
+      <c r="C293" s="13"/>
+      <c r="D293" s="13"/>
     </row>
     <row r="294" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A294" s="5"/>
@@ -23292,62 +23422,80 @@
       <c r="D298" s="14"/>
     </row>
     <row r="299" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A299" s="6"/>
+      <c r="A299" s="5"/>
       <c r="B299" s="6"/>
       <c r="C299" s="14"/>
       <c r="D299" s="14"/>
     </row>
     <row r="300" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A300" s="6"/>
+      <c r="A300" s="5"/>
       <c r="B300" s="6"/>
       <c r="C300" s="14"/>
       <c r="D300" s="14"/>
     </row>
     <row r="301" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A301" s="6"/>
+      <c r="A301" s="5"/>
       <c r="B301" s="6"/>
       <c r="C301" s="14"/>
       <c r="D301" s="14"/>
     </row>
     <row r="302" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A302" s="79"/>
-      <c r="B302" s="79"/>
-      <c r="C302" s="80"/>
-      <c r="D302" s="80"/>
+      <c r="A302" s="6"/>
+      <c r="B302" s="6"/>
+      <c r="C302" s="14"/>
+      <c r="D302" s="14"/>
     </row>
     <row r="303" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A303" s="79"/>
-      <c r="B303" s="79"/>
-      <c r="C303" s="80"/>
-      <c r="D303" s="80"/>
-    </row>
-    <row r="304" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="7"/>
-      <c r="B304" s="7"/>
-      <c r="C304" s="15"/>
-      <c r="D304" s="15"/>
-    </row>
-    <row r="305" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A305" s="76" t="s">
+      <c r="A303" s="6"/>
+      <c r="B303" s="6"/>
+      <c r="C303" s="14"/>
+      <c r="D303" s="14"/>
+    </row>
+    <row r="304" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A304" s="6"/>
+      <c r="B304" s="6"/>
+      <c r="C304" s="14"/>
+      <c r="D304" s="14"/>
+    </row>
+    <row r="305" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A305" s="79"/>
+      <c r="B305" s="79"/>
+      <c r="C305" s="80"/>
+      <c r="D305" s="80"/>
+    </row>
+    <row r="306" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A306" s="79"/>
+      <c r="B306" s="79"/>
+      <c r="C306" s="80"/>
+      <c r="D306" s="80"/>
+    </row>
+    <row r="307" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="7"/>
+      <c r="B307" s="7"/>
+      <c r="C307" s="15"/>
+      <c r="D307" s="15"/>
+    </row>
+    <row r="308" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B305" s="76">
-        <f>SUM(B290:B304)</f>
+      <c r="B308" s="76">
+        <f>SUM(B293:B307)</f>
         <v>0</v>
       </c>
-      <c r="C305" s="107" t="s">
+      <c r="C308" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D305" s="77"/>
-    </row>
-    <row r="306" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A306" s="78"/>
-      <c r="B306" s="78"/>
-      <c r="C306" s="78"/>
-      <c r="D306" s="78"/>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A307" s="106" t="s">
+      <c r="D308" s="77"/>
+    </row>
+    <row r="309" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A309" s="78"/>
+      <c r="B309" s="78"/>
+      <c r="C309" s="78"/>
+      <c r="D309" s="78"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310" s="106" t="s">
         <v>46</v>
       </c>
     </row>
@@ -23357,14 +23505,14 @@
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F27:F34 B3:B17 B22:B36 B41:B56 B61:B75 B80:B95 B100:B114 B119:B133 B138:B152 B157:B171 B176:B190 B195:B209 B214:B228 B233:B247 B252:B266 B271:B285 B290:B304">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F27:F34 B3:B17 B22:B36 B41:B56 B61:B75 B80:B95 B100:B114 B119:B133 B138:B155 B160:B174 B179:B193 B198:B212 B217:B231 B236:B250 B255:B269 B274:B288 B293:B307">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B37 B57 B76 B96 B115 B134 B153 B172 B191 B210 B229 B248 B267 B286 B305">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B37 B57 B76 B96 B115 B134 B156 B175 B194 B213 B232 B251 B270 B289 B308">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A22:A36 A41:A56 A61:A75 A80:A95 A100:A114 A119:A133 A138:A152 A157:A171 A176:A190 A195:A209 A214:A228 A233:A247 A252:A266 A271:A285 A290:A304">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A22:A36 A41:A56 A61:A75 A80:A95 A100:A114 A119:A133 A138:A155 A160:A174 A179:A193 A198:A212 A217:A231 A236:A250 A255:A269 A274:A288 A293:A307">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -23392,21 +23540,24 @@
     <hyperlink ref="D67" r:id="rId21"/>
     <hyperlink ref="D119" r:id="rId22"/>
     <hyperlink ref="D123" r:id="rId23"/>
+    <hyperlink ref="D141" r:id="rId24"/>
+    <hyperlink ref="D140" r:id="rId25"/>
+    <hyperlink ref="D142" r:id="rId26"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" cellComments="atEnd" r:id="rId24"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" cellComments="atEnd" r:id="rId27"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"&amp;24ETML</oddHeader>
     <oddFooter>&amp;C&amp;F&amp;L&amp;D</oddFooter>
   </headerFooter>
-  <drawing r:id="rId25"/>
-  <legacyDrawing r:id="rId26"/>
+  <drawing r:id="rId28"/>
+  <legacyDrawing r:id="rId29"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="44033" r:id="rId27" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+        <control shapeId="44033" r:id="rId30" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -23425,7 +23576,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="44033" r:id="rId27" name="btnImportRealisation"/>
+        <control shapeId="44033" r:id="rId30" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
MAJ JDT + DailyScrum + Probleme.docx
</commit_message>
<xml_diff>
--- a/doc/DemoMotJDT-pittierfa.xlsx
+++ b/doc/DemoMotJDT-pittierfa.xlsx
@@ -36,7 +36,7 @@
     <definedName name="objRealizedWeek" localSheetId="7">JNLTRAV!$A$1:$D$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Diagramme!$A$1:$PT$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$309</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JNLTRAV!$A$1:$D$297</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Planning!$A$1:$D$224</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="134">
   <si>
     <t>Module :</t>
   </si>
@@ -453,7 +453,22 @@
     <t>(Commit pour les branches FPR02 et DEV01 mais checkout entre les branches long car DEV01 contient tout typo3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mise au propre du doccument </t>
+    <t>Examens d'allemand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise au propre du document </t>
+  </si>
+  <si>
+    <t>Problème: Recherche comment utiliser sur notre site l'extension que nous avons crée. (Problème 4)</t>
+  </si>
+  <si>
+    <t>Rédaction du problème 4</t>
+  </si>
+  <si>
+    <t>Avec jimmy on essaie plusieurs façons pour que l'utilisateur puisse publier un jeu depuis le site et que les jeux crées s'affichent dans la page d'accueil (l'utilisateur peut pour le moment juste créer le post mais le jeu et l'user ne sont pas repris)</t>
+  </si>
+  <si>
+    <t>Commit du jour</t>
   </si>
 </sst>
 </file>
@@ -670,7 +685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1299,6 +1314,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1309,7 +1337,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1651,6 +1679,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -20753,10 +20805,10 @@
   <sheetPr codeName="Feuil9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I310"/>
+  <dimension ref="A1:I298"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A138" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A157" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22186,8 +22238,12 @@
       <c r="B138" s="8">
         <v>1</v>
       </c>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
+      <c r="C138" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D138" s="109" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="139" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
@@ -22256,33 +22312,33 @@
       <c r="D143" s="108"/>
     </row>
     <row r="144" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A144" s="5" t="s">
+      <c r="A144" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="111">
         <v>3</v>
       </c>
-      <c r="C144" s="14" t="s">
+      <c r="C144" s="112" t="s">
         <v>118</v>
       </c>
       <c r="D144" s="14"/>
     </row>
     <row r="145" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A145" s="5"/>
-      <c r="B145" s="6"/>
-      <c r="C145" s="14" t="s">
+      <c r="A145" s="113"/>
+      <c r="B145" s="114"/>
+      <c r="C145" s="115" t="s">
         <v>78</v>
       </c>
       <c r="D145" s="14"/>
     </row>
     <row r="146" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A146" s="5" t="s">
+      <c r="A146" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="117">
         <v>4</v>
       </c>
-      <c r="C146" s="14" t="s">
+      <c r="C146" s="118" t="s">
         <v>125</v>
       </c>
       <c r="D146" s="14"/>
@@ -22307,9 +22363,11 @@
         <v>1</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D148" s="14"/>
+        <v>129</v>
+      </c>
+      <c r="D148" s="108" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="149" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
@@ -22324,21 +22382,21 @@
       <c r="D149" s="14"/>
     </row>
     <row r="150" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="79">
         <v>1</v>
       </c>
-      <c r="C150" s="14" t="s">
+      <c r="C150" s="80" t="s">
         <v>127</v>
       </c>
       <c r="D150" s="14"/>
     </row>
     <row r="151" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A151" s="6"/>
-      <c r="B151" s="6"/>
-      <c r="C151" s="14"/>
+      <c r="A151" s="117"/>
+      <c r="B151" s="117"/>
+      <c r="C151" s="118"/>
       <c r="D151" s="14"/>
     </row>
     <row r="152" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -22419,9 +22477,15 @@
       </c>
     </row>
     <row r="160" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A160" s="9"/>
-      <c r="B160" s="8"/>
-      <c r="C160" s="13"/>
+      <c r="A160" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B160" s="8">
+        <v>27</v>
+      </c>
+      <c r="C160" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="D160" s="13"/>
     </row>
     <row r="161" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -22430,186 +22494,249 @@
       <c r="C161" s="14"/>
       <c r="D161" s="14"/>
     </row>
-    <row r="162" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="6"/>
       <c r="C162" s="14"/>
       <c r="D162" s="14"/>
     </row>
-    <row r="163" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A163" s="5"/>
-      <c r="B163" s="6"/>
-      <c r="C163" s="14"/>
-      <c r="D163" s="14"/>
-    </row>
-    <row r="164" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A164" s="5"/>
-      <c r="B164" s="6"/>
-      <c r="C164" s="14"/>
-      <c r="D164" s="14"/>
-    </row>
-    <row r="165" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A165" s="5"/>
-      <c r="B165" s="6"/>
-      <c r="C165" s="14"/>
-      <c r="D165" s="14"/>
-    </row>
-    <row r="166" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A166" s="5"/>
-      <c r="B166" s="6"/>
-      <c r="C166" s="14"/>
-      <c r="D166" s="14"/>
+    <row r="163" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163" s="76">
+        <f>SUM(B160:B162)</f>
+        <v>27</v>
+      </c>
+      <c r="C163" s="107" t="s">
+        <v>45</v>
+      </c>
+      <c r="D163" s="77"/>
+    </row>
+    <row r="164" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="78"/>
+      <c r="B164" s="78"/>
+      <c r="C164" s="78"/>
+      <c r="D164" s="78"/>
+    </row>
+    <row r="165" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" s="72">
+        <v>10</v>
+      </c>
+      <c r="C165" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D165" s="82">
+        <v>42900</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C166" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="74" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="167" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A167" s="5"/>
-      <c r="B167" s="6"/>
-      <c r="C167" s="14"/>
-      <c r="D167" s="14"/>
+      <c r="A167" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B167" s="8">
+        <v>1</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D167" s="109" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="168" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="5"/>
-      <c r="B168" s="6"/>
-      <c r="C168" s="14"/>
-      <c r="D168" s="14"/>
-    </row>
-    <row r="169" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A169" s="6"/>
-      <c r="B169" s="6"/>
-      <c r="C169" s="14"/>
+      <c r="A168" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B168" s="6">
+        <v>2</v>
+      </c>
+      <c r="C168" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D168" s="108" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A169" s="110" t="s">
+        <v>58</v>
+      </c>
+      <c r="B169" s="111">
+        <v>12</v>
+      </c>
+      <c r="C169" s="112" t="s">
+        <v>130</v>
+      </c>
       <c r="D169" s="14"/>
     </row>
     <row r="170" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A170" s="6"/>
-      <c r="B170" s="6"/>
-      <c r="C170" s="14"/>
+      <c r="A170" s="133"/>
+      <c r="B170" s="134"/>
+      <c r="C170" s="135" t="s">
+        <v>78</v>
+      </c>
       <c r="D170" s="14"/>
     </row>
     <row r="171" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A171" s="6"/>
-      <c r="B171" s="6"/>
-      <c r="C171" s="14"/>
-      <c r="D171" s="14"/>
-    </row>
-    <row r="172" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A172" s="79"/>
-      <c r="B172" s="79"/>
-      <c r="C172" s="80"/>
-      <c r="D172" s="80"/>
+      <c r="A171" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="B171" s="131">
+        <v>2</v>
+      </c>
+      <c r="C171" s="132" t="s">
+        <v>131</v>
+      </c>
+      <c r="D171" s="108" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A172" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B172" s="6">
+        <v>9</v>
+      </c>
+      <c r="C172" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D172" s="14"/>
     </row>
     <row r="173" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A173" s="79"/>
-      <c r="B173" s="79"/>
-      <c r="C173" s="80"/>
-      <c r="D173" s="80"/>
-    </row>
-    <row r="174" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="15"/>
-      <c r="D174" s="15"/>
-    </row>
-    <row r="175" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="76" t="s">
+      <c r="A173" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B173" s="6">
+        <v>1</v>
+      </c>
+      <c r="C173" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D173" s="14"/>
+    </row>
+    <row r="174" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A174" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B174" s="6"/>
+      <c r="C174" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D174" s="14"/>
+    </row>
+    <row r="175" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A175" s="5"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="14"/>
+      <c r="D175" s="14"/>
+    </row>
+    <row r="176" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="14"/>
+      <c r="D176" s="14"/>
+    </row>
+    <row r="177" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="14"/>
+      <c r="D177" s="14"/>
+    </row>
+    <row r="178" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="14"/>
+    </row>
+    <row r="179" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A179" s="79"/>
+      <c r="B179" s="79"/>
+      <c r="C179" s="80"/>
+      <c r="D179" s="80"/>
+    </row>
+    <row r="180" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A180" s="79"/>
+      <c r="B180" s="79"/>
+      <c r="C180" s="80"/>
+      <c r="D180" s="80"/>
+    </row>
+    <row r="181" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="7"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="15"/>
+      <c r="D181" s="15"/>
+    </row>
+    <row r="182" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B175" s="76">
-        <f>SUM(B160:B174)</f>
-        <v>0</v>
-      </c>
-      <c r="C175" s="107" t="s">
+      <c r="B182" s="76">
+        <f>SUM(B167:B181)</f>
+        <v>27</v>
+      </c>
+      <c r="C182" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D175" s="77"/>
-    </row>
-    <row r="176" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="78"/>
-      <c r="B176" s="78"/>
-      <c r="C176" s="78"/>
-      <c r="D176" s="78"/>
-    </row>
-    <row r="177" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="71" t="s">
+      <c r="D182" s="77"/>
+    </row>
+    <row r="183" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="78"/>
+      <c r="B183" s="78"/>
+      <c r="C183" s="78"/>
+      <c r="D183" s="78"/>
+    </row>
+    <row r="184" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B177" s="72">
-        <v>10</v>
-      </c>
-      <c r="C177" s="73" t="s">
+      <c r="B184" s="72">
+        <v>11</v>
+      </c>
+      <c r="C184" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D177" s="82">
-        <v>42900</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="74" t="s">
+      <c r="D184" s="82">
+        <v>42902</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B178" s="75" t="s">
+      <c r="B185" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C178" s="74" t="s">
+      <c r="C185" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D178" s="74" t="s">
+      <c r="D185" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A179" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B179" s="8">
-        <v>1</v>
-      </c>
-      <c r="C179" s="13"/>
-      <c r="D179" s="13"/>
-    </row>
-    <row r="180" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A180" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B180" s="6">
-        <v>2</v>
-      </c>
-      <c r="C180" s="14"/>
-      <c r="D180" s="14"/>
-    </row>
-    <row r="181" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A181" s="5"/>
-      <c r="B181" s="6"/>
-      <c r="C181" s="14"/>
-      <c r="D181" s="14"/>
-    </row>
-    <row r="182" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A182" s="5"/>
-      <c r="B182" s="6"/>
-      <c r="C182" s="14"/>
-      <c r="D182" s="14"/>
-    </row>
-    <row r="183" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A183" s="5"/>
-      <c r="B183" s="6"/>
-      <c r="C183" s="14"/>
-      <c r="D183" s="14"/>
-    </row>
-    <row r="184" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A184" s="5"/>
-      <c r="B184" s="6"/>
-      <c r="C184" s="14"/>
-      <c r="D184" s="14"/>
-    </row>
-    <row r="185" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A185" s="5"/>
-      <c r="B185" s="6"/>
-      <c r="C185" s="14"/>
-      <c r="D185" s="14"/>
-    </row>
     <row r="186" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A186" s="5"/>
-      <c r="B186" s="6"/>
-      <c r="C186" s="14"/>
-      <c r="D186" s="14"/>
+      <c r="A186" s="9"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
     </row>
     <row r="187" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A187" s="5"/>
@@ -22618,135 +22745,135 @@
       <c r="D187" s="14"/>
     </row>
     <row r="188" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A188" s="6"/>
+      <c r="A188" s="5"/>
       <c r="B188" s="6"/>
       <c r="C188" s="14"/>
       <c r="D188" s="14"/>
     </row>
     <row r="189" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A189" s="6"/>
+      <c r="A189" s="5"/>
       <c r="B189" s="6"/>
       <c r="C189" s="14"/>
       <c r="D189" s="14"/>
     </row>
     <row r="190" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A190" s="6"/>
+      <c r="A190" s="5"/>
       <c r="B190" s="6"/>
       <c r="C190" s="14"/>
       <c r="D190" s="14"/>
     </row>
     <row r="191" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A191" s="79"/>
-      <c r="B191" s="79"/>
-      <c r="C191" s="80"/>
-      <c r="D191" s="80"/>
+      <c r="A191" s="5"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="14"/>
+      <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A192" s="79"/>
-      <c r="B192" s="79"/>
-      <c r="C192" s="80"/>
-      <c r="D192" s="80"/>
-    </row>
-    <row r="193" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="7"/>
-      <c r="B193" s="7"/>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-    </row>
-    <row r="194" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="76" t="s">
+      <c r="A192" s="5"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="14"/>
+      <c r="D192" s="14"/>
+    </row>
+    <row r="193" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A193" s="5"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="14"/>
+      <c r="D193" s="14"/>
+    </row>
+    <row r="194" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A194" s="5"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="14"/>
+      <c r="D194" s="14"/>
+    </row>
+    <row r="195" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="14"/>
+      <c r="D195" s="14"/>
+    </row>
+    <row r="196" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="14"/>
+      <c r="D196" s="14"/>
+    </row>
+    <row r="197" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="14"/>
+      <c r="D197" s="14"/>
+    </row>
+    <row r="198" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A198" s="79"/>
+      <c r="B198" s="79"/>
+      <c r="C198" s="80"/>
+      <c r="D198" s="80"/>
+    </row>
+    <row r="199" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A199" s="79"/>
+      <c r="B199" s="79"/>
+      <c r="C199" s="80"/>
+      <c r="D199" s="80"/>
+    </row>
+    <row r="200" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="7"/>
+      <c r="B200" s="7"/>
+      <c r="C200" s="15"/>
+      <c r="D200" s="15"/>
+    </row>
+    <row r="201" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B194" s="76">
-        <f>SUM(B179:B193)</f>
+      <c r="B201" s="76">
+        <f>SUM(B186:B200)</f>
+        <v>0</v>
+      </c>
+      <c r="C201" s="107" t="s">
+        <v>45</v>
+      </c>
+      <c r="D201" s="77"/>
+    </row>
+    <row r="202" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="78"/>
+      <c r="B202" s="78"/>
+      <c r="C202" s="78"/>
+      <c r="D202" s="78"/>
+    </row>
+    <row r="203" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B203" s="72">
+        <v>12</v>
+      </c>
+      <c r="C203" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D203" s="82">
+        <v>42912</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C194" s="107" t="s">
-        <v>45</v>
-      </c>
-      <c r="D194" s="77"/>
-    </row>
-    <row r="195" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="78"/>
-      <c r="B195" s="78"/>
-      <c r="C195" s="78"/>
-      <c r="D195" s="78"/>
-    </row>
-    <row r="196" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B196" s="72">
-        <v>11</v>
-      </c>
-      <c r="C196" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D196" s="82">
-        <v>42902</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B197" s="75" t="s">
+      <c r="B204" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C197" s="74" t="s">
+      <c r="C204" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D197" s="74" t="s">
+      <c r="D204" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A198" s="9"/>
-      <c r="B198" s="8"/>
-      <c r="C198" s="13"/>
-      <c r="D198" s="13"/>
-    </row>
-    <row r="199" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A199" s="5"/>
-      <c r="B199" s="6"/>
-      <c r="C199" s="14"/>
-      <c r="D199" s="14"/>
-    </row>
-    <row r="200" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A200" s="5"/>
-      <c r="B200" s="6"/>
-      <c r="C200" s="14"/>
-      <c r="D200" s="14"/>
-    </row>
-    <row r="201" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A201" s="5"/>
-      <c r="B201" s="6"/>
-      <c r="C201" s="14"/>
-      <c r="D201" s="14"/>
-    </row>
-    <row r="202" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A202" s="5"/>
-      <c r="B202" s="6"/>
-      <c r="C202" s="14"/>
-      <c r="D202" s="14"/>
-    </row>
-    <row r="203" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A203" s="5"/>
-      <c r="B203" s="6"/>
-      <c r="C203" s="14"/>
-      <c r="D203" s="14"/>
-    </row>
-    <row r="204" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A204" s="5"/>
-      <c r="B204" s="6"/>
-      <c r="C204" s="14"/>
-      <c r="D204" s="14"/>
-    </row>
     <row r="205" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A205" s="5"/>
-      <c r="B205" s="6"/>
-      <c r="C205" s="14"/>
-      <c r="D205" s="14"/>
+      <c r="A205" s="9"/>
+      <c r="B205" s="8"/>
+      <c r="C205" s="13"/>
+      <c r="D205" s="13"/>
     </row>
     <row r="206" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A206" s="5"/>
@@ -22755,135 +22882,135 @@
       <c r="D206" s="14"/>
     </row>
     <row r="207" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A207" s="6"/>
+      <c r="A207" s="5"/>
       <c r="B207" s="6"/>
       <c r="C207" s="14"/>
       <c r="D207" s="14"/>
     </row>
     <row r="208" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A208" s="6"/>
+      <c r="A208" s="5"/>
       <c r="B208" s="6"/>
       <c r="C208" s="14"/>
       <c r="D208" s="14"/>
     </row>
     <row r="209" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A209" s="6"/>
+      <c r="A209" s="5"/>
       <c r="B209" s="6"/>
       <c r="C209" s="14"/>
       <c r="D209" s="14"/>
     </row>
     <row r="210" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A210" s="79"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="80"/>
-      <c r="D210" s="80"/>
+      <c r="A210" s="5"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="14"/>
+      <c r="D210" s="14"/>
     </row>
     <row r="211" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A211" s="79"/>
-      <c r="B211" s="79"/>
-      <c r="C211" s="80"/>
-      <c r="D211" s="80"/>
-    </row>
-    <row r="212" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="7"/>
-      <c r="B212" s="7"/>
-      <c r="C212" s="15"/>
-      <c r="D212" s="15"/>
-    </row>
-    <row r="213" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="76" t="s">
+      <c r="A211" s="5"/>
+      <c r="B211" s="6"/>
+      <c r="C211" s="14"/>
+      <c r="D211" s="14"/>
+    </row>
+    <row r="212" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A212" s="5"/>
+      <c r="B212" s="6"/>
+      <c r="C212" s="14"/>
+      <c r="D212" s="14"/>
+    </row>
+    <row r="213" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A213" s="5"/>
+      <c r="B213" s="6"/>
+      <c r="C213" s="14"/>
+      <c r="D213" s="14"/>
+    </row>
+    <row r="214" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A214" s="6"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="14"/>
+      <c r="D214" s="14"/>
+    </row>
+    <row r="215" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A215" s="6"/>
+      <c r="B215" s="6"/>
+      <c r="C215" s="14"/>
+      <c r="D215" s="14"/>
+    </row>
+    <row r="216" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A216" s="6"/>
+      <c r="B216" s="6"/>
+      <c r="C216" s="14"/>
+      <c r="D216" s="14"/>
+    </row>
+    <row r="217" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A217" s="79"/>
+      <c r="B217" s="79"/>
+      <c r="C217" s="80"/>
+      <c r="D217" s="80"/>
+    </row>
+    <row r="218" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A218" s="79"/>
+      <c r="B218" s="79"/>
+      <c r="C218" s="80"/>
+      <c r="D218" s="80"/>
+    </row>
+    <row r="219" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="7"/>
+      <c r="B219" s="7"/>
+      <c r="C219" s="15"/>
+      <c r="D219" s="15"/>
+    </row>
+    <row r="220" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B213" s="76">
-        <f>SUM(B198:B212)</f>
+      <c r="B220" s="76">
+        <f>SUM(B205:B219)</f>
         <v>0</v>
       </c>
-      <c r="C213" s="107" t="s">
+      <c r="C220" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D213" s="77"/>
-    </row>
-    <row r="214" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="78"/>
-      <c r="B214" s="78"/>
-      <c r="C214" s="78"/>
-      <c r="D214" s="78"/>
-    </row>
-    <row r="215" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="71" t="s">
+      <c r="D220" s="77"/>
+    </row>
+    <row r="221" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A221" s="78"/>
+      <c r="B221" s="78"/>
+      <c r="C221" s="78"/>
+      <c r="D221" s="78"/>
+    </row>
+    <row r="222" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B215" s="72">
-        <v>12</v>
-      </c>
-      <c r="C215" s="73" t="s">
+      <c r="B222" s="72">
+        <v>13</v>
+      </c>
+      <c r="C222" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D215" s="82">
-        <v>42912</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="74" t="s">
+      <c r="D222" s="82">
+        <v>42968</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B216" s="75" t="s">
+      <c r="B223" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C216" s="74" t="s">
+      <c r="C223" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D216" s="74" t="s">
+      <c r="D223" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A217" s="9"/>
-      <c r="B217" s="8"/>
-      <c r="C217" s="13"/>
-      <c r="D217" s="13"/>
-    </row>
-    <row r="218" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A218" s="5"/>
-      <c r="B218" s="6"/>
-      <c r="C218" s="14"/>
-      <c r="D218" s="14"/>
-    </row>
-    <row r="219" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A219" s="5"/>
-      <c r="B219" s="6"/>
-      <c r="C219" s="14"/>
-      <c r="D219" s="14"/>
-    </row>
-    <row r="220" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A220" s="5"/>
-      <c r="B220" s="6"/>
-      <c r="C220" s="14"/>
-      <c r="D220" s="14"/>
-    </row>
-    <row r="221" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A221" s="5"/>
-      <c r="B221" s="6"/>
-      <c r="C221" s="14"/>
-      <c r="D221" s="14"/>
-    </row>
-    <row r="222" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A222" s="5"/>
-      <c r="B222" s="6"/>
-      <c r="C222" s="14"/>
-      <c r="D222" s="14"/>
-    </row>
-    <row r="223" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A223" s="5"/>
-      <c r="B223" s="6"/>
-      <c r="C223" s="14"/>
-      <c r="D223" s="14"/>
-    </row>
     <row r="224" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A224" s="5"/>
-      <c r="B224" s="6"/>
-      <c r="C224" s="14"/>
-      <c r="D224" s="14"/>
+      <c r="A224" s="9"/>
+      <c r="B224" s="8"/>
+      <c r="C224" s="13"/>
+      <c r="D224" s="13"/>
     </row>
     <row r="225" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A225" s="5"/>
@@ -22892,135 +23019,135 @@
       <c r="D225" s="14"/>
     </row>
     <row r="226" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A226" s="6"/>
+      <c r="A226" s="5"/>
       <c r="B226" s="6"/>
       <c r="C226" s="14"/>
       <c r="D226" s="14"/>
     </row>
     <row r="227" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A227" s="6"/>
+      <c r="A227" s="5"/>
       <c r="B227" s="6"/>
       <c r="C227" s="14"/>
       <c r="D227" s="14"/>
     </row>
     <row r="228" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A228" s="6"/>
+      <c r="A228" s="5"/>
       <c r="B228" s="6"/>
       <c r="C228" s="14"/>
       <c r="D228" s="14"/>
     </row>
     <row r="229" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A229" s="79"/>
-      <c r="B229" s="79"/>
-      <c r="C229" s="80"/>
-      <c r="D229" s="80"/>
+      <c r="A229" s="5"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="14"/>
+      <c r="D229" s="14"/>
     </row>
     <row r="230" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A230" s="79"/>
-      <c r="B230" s="79"/>
-      <c r="C230" s="80"/>
-      <c r="D230" s="80"/>
-    </row>
-    <row r="231" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="7"/>
-      <c r="B231" s="7"/>
-      <c r="C231" s="15"/>
-      <c r="D231" s="15"/>
-    </row>
-    <row r="232" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="76" t="s">
+      <c r="A230" s="5"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="14"/>
+      <c r="D230" s="14"/>
+    </row>
+    <row r="231" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A231" s="5"/>
+      <c r="B231" s="6"/>
+      <c r="C231" s="14"/>
+      <c r="D231" s="14"/>
+    </row>
+    <row r="232" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A232" s="5"/>
+      <c r="B232" s="6"/>
+      <c r="C232" s="14"/>
+      <c r="D232" s="14"/>
+    </row>
+    <row r="233" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A233" s="6"/>
+      <c r="B233" s="6"/>
+      <c r="C233" s="14"/>
+      <c r="D233" s="14"/>
+    </row>
+    <row r="234" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A234" s="6"/>
+      <c r="B234" s="6"/>
+      <c r="C234" s="14"/>
+      <c r="D234" s="14"/>
+    </row>
+    <row r="235" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A235" s="6"/>
+      <c r="B235" s="6"/>
+      <c r="C235" s="14"/>
+      <c r="D235" s="14"/>
+    </row>
+    <row r="236" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A236" s="79"/>
+      <c r="B236" s="79"/>
+      <c r="C236" s="80"/>
+      <c r="D236" s="80"/>
+    </row>
+    <row r="237" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A237" s="79"/>
+      <c r="B237" s="79"/>
+      <c r="C237" s="80"/>
+      <c r="D237" s="80"/>
+    </row>
+    <row r="238" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="7"/>
+      <c r="B238" s="7"/>
+      <c r="C238" s="15"/>
+      <c r="D238" s="15"/>
+    </row>
+    <row r="239" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B232" s="76">
-        <f>SUM(B217:B231)</f>
+      <c r="B239" s="76">
+        <f>SUM(B224:B238)</f>
         <v>0</v>
       </c>
-      <c r="C232" s="107" t="s">
+      <c r="C239" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D232" s="77"/>
-    </row>
-    <row r="233" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="78"/>
-      <c r="B233" s="78"/>
-      <c r="C233" s="78"/>
-      <c r="D233" s="78"/>
-    </row>
-    <row r="234" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="71" t="s">
+      <c r="D239" s="77"/>
+    </row>
+    <row r="240" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A240" s="78"/>
+      <c r="B240" s="78"/>
+      <c r="C240" s="78"/>
+      <c r="D240" s="78"/>
+    </row>
+    <row r="241" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B234" s="72">
+      <c r="B241" s="72">
+        <v>14</v>
+      </c>
+      <c r="C241" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D241" s="82">
+        <v>42975</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C242" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D242" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C234" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D234" s="82">
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B235" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C235" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D235" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A236" s="9"/>
-      <c r="B236" s="8"/>
-      <c r="C236" s="13"/>
-      <c r="D236" s="13"/>
-    </row>
-    <row r="237" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A237" s="5"/>
-      <c r="B237" s="6"/>
-      <c r="C237" s="14"/>
-      <c r="D237" s="14"/>
-    </row>
-    <row r="238" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A238" s="5"/>
-      <c r="B238" s="6"/>
-      <c r="C238" s="14"/>
-      <c r="D238" s="14"/>
-    </row>
-    <row r="239" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A239" s="5"/>
-      <c r="B239" s="6"/>
-      <c r="C239" s="14"/>
-      <c r="D239" s="14"/>
-    </row>
-    <row r="240" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A240" s="5"/>
-      <c r="B240" s="6"/>
-      <c r="C240" s="14"/>
-      <c r="D240" s="14"/>
-    </row>
-    <row r="241" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A241" s="5"/>
-      <c r="B241" s="6"/>
-      <c r="C241" s="14"/>
-      <c r="D241" s="14"/>
-    </row>
-    <row r="242" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A242" s="5"/>
-      <c r="B242" s="6"/>
-      <c r="C242" s="14"/>
-      <c r="D242" s="14"/>
     </row>
     <row r="243" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A243" s="5"/>
-      <c r="B243" s="6"/>
-      <c r="C243" s="14"/>
-      <c r="D243" s="14"/>
+      <c r="A243" s="9"/>
+      <c r="B243" s="8"/>
+      <c r="C243" s="13"/>
+      <c r="D243" s="13"/>
     </row>
     <row r="244" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A244" s="5"/>
@@ -23029,135 +23156,135 @@
       <c r="D244" s="14"/>
     </row>
     <row r="245" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A245" s="6"/>
+      <c r="A245" s="5"/>
       <c r="B245" s="6"/>
       <c r="C245" s="14"/>
       <c r="D245" s="14"/>
     </row>
     <row r="246" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A246" s="6"/>
+      <c r="A246" s="5"/>
       <c r="B246" s="6"/>
       <c r="C246" s="14"/>
       <c r="D246" s="14"/>
     </row>
     <row r="247" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A247" s="6"/>
+      <c r="A247" s="5"/>
       <c r="B247" s="6"/>
       <c r="C247" s="14"/>
       <c r="D247" s="14"/>
     </row>
     <row r="248" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A248" s="79"/>
-      <c r="B248" s="79"/>
-      <c r="C248" s="80"/>
-      <c r="D248" s="80"/>
+      <c r="A248" s="5"/>
+      <c r="B248" s="6"/>
+      <c r="C248" s="14"/>
+      <c r="D248" s="14"/>
     </row>
     <row r="249" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A249" s="79"/>
-      <c r="B249" s="79"/>
-      <c r="C249" s="80"/>
-      <c r="D249" s="80"/>
-    </row>
-    <row r="250" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="7"/>
-      <c r="B250" s="7"/>
-      <c r="C250" s="15"/>
-      <c r="D250" s="15"/>
-    </row>
-    <row r="251" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="76" t="s">
+      <c r="A249" s="5"/>
+      <c r="B249" s="6"/>
+      <c r="C249" s="14"/>
+      <c r="D249" s="14"/>
+    </row>
+    <row r="250" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A250" s="5"/>
+      <c r="B250" s="6"/>
+      <c r="C250" s="14"/>
+      <c r="D250" s="14"/>
+    </row>
+    <row r="251" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A251" s="5"/>
+      <c r="B251" s="6"/>
+      <c r="C251" s="14"/>
+      <c r="D251" s="14"/>
+    </row>
+    <row r="252" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A252" s="6"/>
+      <c r="B252" s="6"/>
+      <c r="C252" s="14"/>
+      <c r="D252" s="14"/>
+    </row>
+    <row r="253" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A253" s="6"/>
+      <c r="B253" s="6"/>
+      <c r="C253" s="14"/>
+      <c r="D253" s="14"/>
+    </row>
+    <row r="254" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A254" s="6"/>
+      <c r="B254" s="6"/>
+      <c r="C254" s="14"/>
+      <c r="D254" s="14"/>
+    </row>
+    <row r="255" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A255" s="79"/>
+      <c r="B255" s="79"/>
+      <c r="C255" s="80"/>
+      <c r="D255" s="80"/>
+    </row>
+    <row r="256" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A256" s="79"/>
+      <c r="B256" s="79"/>
+      <c r="C256" s="80"/>
+      <c r="D256" s="80"/>
+    </row>
+    <row r="257" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="7"/>
+      <c r="B257" s="7"/>
+      <c r="C257" s="15"/>
+      <c r="D257" s="15"/>
+    </row>
+    <row r="258" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B251" s="76">
-        <f>SUM(B236:B250)</f>
+      <c r="B258" s="76">
+        <f>SUM(B243:B257)</f>
         <v>0</v>
       </c>
-      <c r="C251" s="107" t="s">
+      <c r="C258" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D251" s="77"/>
-    </row>
-    <row r="252" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A252" s="78"/>
-      <c r="B252" s="78"/>
-      <c r="C252" s="78"/>
-      <c r="D252" s="78"/>
-    </row>
-    <row r="253" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="71" t="s">
+      <c r="D258" s="77"/>
+    </row>
+    <row r="259" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A259" s="78"/>
+      <c r="B259" s="78"/>
+      <c r="C259" s="78"/>
+      <c r="D259" s="78"/>
+    </row>
+    <row r="260" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B253" s="72">
-        <v>14</v>
-      </c>
-      <c r="C253" s="73" t="s">
+      <c r="B260" s="72">
+        <v>15</v>
+      </c>
+      <c r="C260" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D253" s="82">
-        <v>42975</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="74" t="s">
+      <c r="D260" s="82">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B254" s="75" t="s">
+      <c r="B261" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C254" s="74" t="s">
+      <c r="C261" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D254" s="74" t="s">
+      <c r="D261" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A255" s="9"/>
-      <c r="B255" s="8"/>
-      <c r="C255" s="13"/>
-      <c r="D255" s="13"/>
-    </row>
-    <row r="256" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A256" s="5"/>
-      <c r="B256" s="6"/>
-      <c r="C256" s="14"/>
-      <c r="D256" s="14"/>
-    </row>
-    <row r="257" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A257" s="5"/>
-      <c r="B257" s="6"/>
-      <c r="C257" s="14"/>
-      <c r="D257" s="14"/>
-    </row>
-    <row r="258" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A258" s="5"/>
-      <c r="B258" s="6"/>
-      <c r="C258" s="14"/>
-      <c r="D258" s="14"/>
-    </row>
-    <row r="259" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A259" s="5"/>
-      <c r="B259" s="6"/>
-      <c r="C259" s="14"/>
-      <c r="D259" s="14"/>
-    </row>
-    <row r="260" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A260" s="5"/>
-      <c r="B260" s="6"/>
-      <c r="C260" s="14"/>
-      <c r="D260" s="14"/>
-    </row>
-    <row r="261" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A261" s="5"/>
-      <c r="B261" s="6"/>
-      <c r="C261" s="14"/>
-      <c r="D261" s="14"/>
-    </row>
     <row r="262" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A262" s="5"/>
-      <c r="B262" s="6"/>
-      <c r="C262" s="14"/>
-      <c r="D262" s="14"/>
+      <c r="A262" s="9"/>
+      <c r="B262" s="8"/>
+      <c r="C262" s="13"/>
+      <c r="D262" s="13"/>
     </row>
     <row r="263" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A263" s="5"/>
@@ -23166,135 +23293,135 @@
       <c r="D263" s="14"/>
     </row>
     <row r="264" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A264" s="6"/>
+      <c r="A264" s="5"/>
       <c r="B264" s="6"/>
       <c r="C264" s="14"/>
       <c r="D264" s="14"/>
     </row>
     <row r="265" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A265" s="6"/>
+      <c r="A265" s="5"/>
       <c r="B265" s="6"/>
       <c r="C265" s="14"/>
       <c r="D265" s="14"/>
     </row>
     <row r="266" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A266" s="6"/>
+      <c r="A266" s="5"/>
       <c r="B266" s="6"/>
       <c r="C266" s="14"/>
       <c r="D266" s="14"/>
     </row>
     <row r="267" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A267" s="79"/>
-      <c r="B267" s="79"/>
-      <c r="C267" s="80"/>
-      <c r="D267" s="80"/>
+      <c r="A267" s="5"/>
+      <c r="B267" s="6"/>
+      <c r="C267" s="14"/>
+      <c r="D267" s="14"/>
     </row>
     <row r="268" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A268" s="79"/>
-      <c r="B268" s="79"/>
-      <c r="C268" s="80"/>
-      <c r="D268" s="80"/>
-    </row>
-    <row r="269" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="7"/>
-      <c r="B269" s="7"/>
-      <c r="C269" s="15"/>
-      <c r="D269" s="15"/>
-    </row>
-    <row r="270" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="76" t="s">
+      <c r="A268" s="5"/>
+      <c r="B268" s="6"/>
+      <c r="C268" s="14"/>
+      <c r="D268" s="14"/>
+    </row>
+    <row r="269" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A269" s="5"/>
+      <c r="B269" s="6"/>
+      <c r="C269" s="14"/>
+      <c r="D269" s="14"/>
+    </row>
+    <row r="270" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A270" s="5"/>
+      <c r="B270" s="6"/>
+      <c r="C270" s="14"/>
+      <c r="D270" s="14"/>
+    </row>
+    <row r="271" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A271" s="6"/>
+      <c r="B271" s="6"/>
+      <c r="C271" s="14"/>
+      <c r="D271" s="14"/>
+    </row>
+    <row r="272" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A272" s="6"/>
+      <c r="B272" s="6"/>
+      <c r="C272" s="14"/>
+      <c r="D272" s="14"/>
+    </row>
+    <row r="273" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A273" s="6"/>
+      <c r="B273" s="6"/>
+      <c r="C273" s="14"/>
+      <c r="D273" s="14"/>
+    </row>
+    <row r="274" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A274" s="79"/>
+      <c r="B274" s="79"/>
+      <c r="C274" s="80"/>
+      <c r="D274" s="80"/>
+    </row>
+    <row r="275" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A275" s="79"/>
+      <c r="B275" s="79"/>
+      <c r="C275" s="80"/>
+      <c r="D275" s="80"/>
+    </row>
+    <row r="276" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="7"/>
+      <c r="B276" s="7"/>
+      <c r="C276" s="15"/>
+      <c r="D276" s="15"/>
+    </row>
+    <row r="277" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B270" s="76">
-        <f>SUM(B255:B269)</f>
+      <c r="B277" s="76">
+        <f>SUM(B262:B276)</f>
         <v>0</v>
       </c>
-      <c r="C270" s="107" t="s">
+      <c r="C277" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D270" s="77"/>
-    </row>
-    <row r="271" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A271" s="78"/>
-      <c r="B271" s="78"/>
-      <c r="C271" s="78"/>
-      <c r="D271" s="78"/>
-    </row>
-    <row r="272" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="71" t="s">
+      <c r="D277" s="77"/>
+    </row>
+    <row r="278" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A278" s="78"/>
+      <c r="B278" s="78"/>
+      <c r="C278" s="78"/>
+      <c r="D278" s="78"/>
+    </row>
+    <row r="279" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B272" s="72">
+      <c r="B279" s="72">
+        <v>16</v>
+      </c>
+      <c r="C279" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D279" s="82">
+        <v>42989</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C272" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D272" s="82">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B273" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C273" s="74" t="s">
+      <c r="C280" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D273" s="74" t="s">
+      <c r="D280" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A274" s="9"/>
-      <c r="B274" s="8"/>
-      <c r="C274" s="13"/>
-      <c r="D274" s="13"/>
-    </row>
-    <row r="275" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A275" s="5"/>
-      <c r="B275" s="6"/>
-      <c r="C275" s="14"/>
-      <c r="D275" s="14"/>
-    </row>
-    <row r="276" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A276" s="5"/>
-      <c r="B276" s="6"/>
-      <c r="C276" s="14"/>
-      <c r="D276" s="14"/>
-    </row>
-    <row r="277" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A277" s="5"/>
-      <c r="B277" s="6"/>
-      <c r="C277" s="14"/>
-      <c r="D277" s="14"/>
-    </row>
-    <row r="278" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A278" s="5"/>
-      <c r="B278" s="6"/>
-      <c r="C278" s="14"/>
-      <c r="D278" s="14"/>
-    </row>
-    <row r="279" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A279" s="5"/>
-      <c r="B279" s="6"/>
-      <c r="C279" s="14"/>
-      <c r="D279" s="14"/>
-    </row>
-    <row r="280" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A280" s="5"/>
-      <c r="B280" s="6"/>
-      <c r="C280" s="14"/>
-      <c r="D280" s="14"/>
-    </row>
     <row r="281" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A281" s="5"/>
-      <c r="B281" s="6"/>
-      <c r="C281" s="14"/>
-      <c r="D281" s="14"/>
+      <c r="A281" s="9"/>
+      <c r="B281" s="8"/>
+      <c r="C281" s="13"/>
+      <c r="D281" s="13"/>
     </row>
     <row r="282" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A282" s="5"/>
@@ -23303,199 +23430,104 @@
       <c r="D282" s="14"/>
     </row>
     <row r="283" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A283" s="6"/>
+      <c r="A283" s="5"/>
       <c r="B283" s="6"/>
       <c r="C283" s="14"/>
       <c r="D283" s="14"/>
     </row>
     <row r="284" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A284" s="6"/>
+      <c r="A284" s="5"/>
       <c r="B284" s="6"/>
       <c r="C284" s="14"/>
       <c r="D284" s="14"/>
     </row>
     <row r="285" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A285" s="6"/>
+      <c r="A285" s="5"/>
       <c r="B285" s="6"/>
       <c r="C285" s="14"/>
       <c r="D285" s="14"/>
     </row>
     <row r="286" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A286" s="79"/>
-      <c r="B286" s="79"/>
-      <c r="C286" s="80"/>
-      <c r="D286" s="80"/>
+      <c r="A286" s="5"/>
+      <c r="B286" s="6"/>
+      <c r="C286" s="14"/>
+      <c r="D286" s="14"/>
     </row>
     <row r="287" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A287" s="79"/>
-      <c r="B287" s="79"/>
-      <c r="C287" s="80"/>
-      <c r="D287" s="80"/>
-    </row>
-    <row r="288" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="7"/>
-      <c r="B288" s="7"/>
-      <c r="C288" s="15"/>
-      <c r="D288" s="15"/>
-    </row>
-    <row r="289" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="76" t="s">
+      <c r="A287" s="5"/>
+      <c r="B287" s="6"/>
+      <c r="C287" s="14"/>
+      <c r="D287" s="14"/>
+    </row>
+    <row r="288" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A288" s="5"/>
+      <c r="B288" s="6"/>
+      <c r="C288" s="14"/>
+      <c r="D288" s="14"/>
+    </row>
+    <row r="289" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A289" s="5"/>
+      <c r="B289" s="6"/>
+      <c r="C289" s="14"/>
+      <c r="D289" s="14"/>
+    </row>
+    <row r="290" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A290" s="6"/>
+      <c r="B290" s="6"/>
+      <c r="C290" s="14"/>
+      <c r="D290" s="14"/>
+    </row>
+    <row r="291" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A291" s="6"/>
+      <c r="B291" s="6"/>
+      <c r="C291" s="14"/>
+      <c r="D291" s="14"/>
+    </row>
+    <row r="292" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A292" s="6"/>
+      <c r="B292" s="6"/>
+      <c r="C292" s="14"/>
+      <c r="D292" s="14"/>
+    </row>
+    <row r="293" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A293" s="79"/>
+      <c r="B293" s="79"/>
+      <c r="C293" s="80"/>
+      <c r="D293" s="80"/>
+    </row>
+    <row r="294" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A294" s="79"/>
+      <c r="B294" s="79"/>
+      <c r="C294" s="80"/>
+      <c r="D294" s="80"/>
+    </row>
+    <row r="295" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="7"/>
+      <c r="B295" s="7"/>
+      <c r="C295" s="15"/>
+      <c r="D295" s="15"/>
+    </row>
+    <row r="296" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B289" s="76">
-        <f>SUM(B274:B288)</f>
+      <c r="B296" s="76">
+        <f>SUM(B281:B295)</f>
         <v>0</v>
       </c>
-      <c r="C289" s="107" t="s">
+      <c r="C296" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D289" s="77"/>
-    </row>
-    <row r="290" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A290" s="78"/>
-      <c r="B290" s="78"/>
-      <c r="C290" s="78"/>
-      <c r="D290" s="78"/>
-    </row>
-    <row r="291" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B291" s="72">
-        <v>16</v>
-      </c>
-      <c r="C291" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D291" s="82">
-        <v>42989</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B292" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C292" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D292" s="74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A293" s="9"/>
-      <c r="B293" s="8"/>
-      <c r="C293" s="13"/>
-      <c r="D293" s="13"/>
-    </row>
-    <row r="294" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A294" s="5"/>
-      <c r="B294" s="6"/>
-      <c r="C294" s="14"/>
-      <c r="D294" s="14"/>
-    </row>
-    <row r="295" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A295" s="5"/>
-      <c r="B295" s="6"/>
-      <c r="C295" s="14"/>
-      <c r="D295" s="14"/>
-    </row>
-    <row r="296" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A296" s="5"/>
-      <c r="B296" s="6"/>
-      <c r="C296" s="14"/>
-      <c r="D296" s="14"/>
-    </row>
-    <row r="297" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A297" s="5"/>
-      <c r="B297" s="6"/>
-      <c r="C297" s="14"/>
-      <c r="D297" s="14"/>
-    </row>
-    <row r="298" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A298" s="5"/>
-      <c r="B298" s="6"/>
-      <c r="C298" s="14"/>
-      <c r="D298" s="14"/>
-    </row>
-    <row r="299" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A299" s="5"/>
-      <c r="B299" s="6"/>
-      <c r="C299" s="14"/>
-      <c r="D299" s="14"/>
-    </row>
-    <row r="300" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A300" s="5"/>
-      <c r="B300" s="6"/>
-      <c r="C300" s="14"/>
-      <c r="D300" s="14"/>
-    </row>
-    <row r="301" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A301" s="5"/>
-      <c r="B301" s="6"/>
-      <c r="C301" s="14"/>
-      <c r="D301" s="14"/>
-    </row>
-    <row r="302" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A302" s="6"/>
-      <c r="B302" s="6"/>
-      <c r="C302" s="14"/>
-      <c r="D302" s="14"/>
-    </row>
-    <row r="303" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A303" s="6"/>
-      <c r="B303" s="6"/>
-      <c r="C303" s="14"/>
-      <c r="D303" s="14"/>
-    </row>
-    <row r="304" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A304" s="6"/>
-      <c r="B304" s="6"/>
-      <c r="C304" s="14"/>
-      <c r="D304" s="14"/>
-    </row>
-    <row r="305" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A305" s="79"/>
-      <c r="B305" s="79"/>
-      <c r="C305" s="80"/>
-      <c r="D305" s="80"/>
-    </row>
-    <row r="306" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A306" s="79"/>
-      <c r="B306" s="79"/>
-      <c r="C306" s="80"/>
-      <c r="D306" s="80"/>
-    </row>
-    <row r="307" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="7"/>
-      <c r="B307" s="7"/>
-      <c r="C307" s="15"/>
-      <c r="D307" s="15"/>
-    </row>
-    <row r="308" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="B308" s="76">
-        <f>SUM(B293:B307)</f>
-        <v>0</v>
-      </c>
-      <c r="C308" s="107" t="s">
-        <v>45</v>
-      </c>
-      <c r="D308" s="77"/>
-    </row>
-    <row r="309" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A309" s="78"/>
-      <c r="B309" s="78"/>
-      <c r="C309" s="78"/>
-      <c r="D309" s="78"/>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A310" s="106" t="s">
+      <c r="D296" s="77"/>
+    </row>
+    <row r="297" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A297" s="78"/>
+      <c r="B297" s="78"/>
+      <c r="C297" s="78"/>
+      <c r="D297" s="78"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298" s="106" t="s">
         <v>46</v>
       </c>
     </row>
@@ -23505,14 +23537,14 @@
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F27:F34 B3:B17 B22:B36 B41:B56 B61:B75 B80:B95 B100:B114 B119:B133 B138:B155 B160:B174 B179:B193 B198:B212 B217:B231 B236:B250 B255:B269 B274:B288 B293:B307">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F27:F34 B3:B17 B22:B36 B41:B56 B61:B75 B80:B95 B100:B114 B119:B133 B138:B155 B160:B162 B167:B181 B186:B200 B205:B219 B224:B238 B243:B257 B262:B276 B281:B295">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B37 B57 B76 B96 B115 B134 B156 B175 B194 B213 B232 B251 B270 B289 B308">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B37 B57 B76 B96 B115 B134 B156 B163 B182 B201 B220 B239 B258 B277 B296">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A22:A36 A41:A56 A61:A75 A80:A95 A100:A114 A119:A133 A138:A155 A160:A174 A179:A193 A198:A212 A217:A231 A236:A250 A255:A269 A274:A288 A293:A307">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A22:A36 A41:A56 A61:A75 A80:A95 A100:A114 A119:A133 A138:A155 A160:A162 A167:A181 A186:A200 A205:A219 A224:A238 A243:A257 A262:A276 A281:A295">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -23543,21 +23575,26 @@
     <hyperlink ref="D141" r:id="rId24"/>
     <hyperlink ref="D140" r:id="rId25"/>
     <hyperlink ref="D142" r:id="rId26"/>
+    <hyperlink ref="D138" r:id="rId27"/>
+    <hyperlink ref="D148" r:id="rId28"/>
+    <hyperlink ref="D167" r:id="rId29"/>
+    <hyperlink ref="D168" r:id="rId30"/>
+    <hyperlink ref="D171" r:id="rId31"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" cellComments="atEnd" r:id="rId27"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" cellComments="atEnd" r:id="rId32"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"&amp;24ETML</oddHeader>
     <oddFooter>&amp;C&amp;F&amp;L&amp;D</oddFooter>
   </headerFooter>
-  <drawing r:id="rId28"/>
-  <legacyDrawing r:id="rId29"/>
+  <drawing r:id="rId33"/>
+  <legacyDrawing r:id="rId34"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="44033" r:id="rId30" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
+        <control shapeId="44033" r:id="rId35" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId36">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -23576,7 +23613,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="44033" r:id="rId30" name="btnImportRealisation"/>
+        <control shapeId="44033" r:id="rId35" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
MAJ JDT + DailyScrum 16.06.17 v.FPR
</commit_message>
<xml_diff>
--- a/doc/DemoMotJDT-pittierfa.xlsx
+++ b/doc/DemoMotJDT-pittierfa.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="139">
   <si>
     <t>Module :</t>
   </si>
@@ -469,6 +469,21 @@
   </si>
   <si>
     <t>Commit du jour</t>
+  </si>
+  <si>
+    <t>Prof parle</t>
+  </si>
+  <si>
+    <t>change l'affichage par défaut des jeux publiés. Téléchargement du Jeux quand cliqué sur son nom, traduction en français</t>
+  </si>
+  <si>
+    <t>Pause midi</t>
+  </si>
+  <si>
+    <t>ajoute bouton d'upload dans formulaire création d'un jeu, path du jeu (chemin du jeu) généré automatiquement mais il y a une erreur qui est cachée car logs désactivé sur easy php -&gt; télécharge et install xdebug mais pas de changements</t>
+  </si>
+  <si>
+    <t>Apéro de section</t>
   </si>
 </sst>
 </file>
@@ -1650,6 +1665,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1679,30 +1718,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2610,10 +2625,10 @@
     </row>
     <row r="19" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="120"/>
+      <c r="C19" s="126"/>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
@@ -3571,474 +3586,474 @@
       <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="121" t="s">
+      <c r="D2" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
-      <c r="R2" s="122"/>
-      <c r="S2" s="122"/>
-      <c r="T2" s="122"/>
-      <c r="U2" s="122"/>
-      <c r="V2" s="122"/>
-      <c r="W2" s="122"/>
-      <c r="X2" s="122"/>
-      <c r="Y2" s="122"/>
-      <c r="Z2" s="122"/>
-      <c r="AA2" s="122"/>
-      <c r="AB2" s="122"/>
-      <c r="AC2" s="122"/>
-      <c r="AD2" s="123"/>
-      <c r="AE2" s="121" t="s">
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="128"/>
+      <c r="Q2" s="128"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="128"/>
+      <c r="W2" s="128"/>
+      <c r="X2" s="128"/>
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="128"/>
+      <c r="AA2" s="128"/>
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="128"/>
+      <c r="AD2" s="129"/>
+      <c r="AE2" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="122"/>
-      <c r="AG2" s="122"/>
-      <c r="AH2" s="122"/>
-      <c r="AI2" s="122"/>
-      <c r="AJ2" s="122"/>
-      <c r="AK2" s="122"/>
-      <c r="AL2" s="122"/>
-      <c r="AM2" s="122"/>
-      <c r="AN2" s="122"/>
-      <c r="AO2" s="122"/>
-      <c r="AP2" s="122"/>
-      <c r="AQ2" s="122"/>
-      <c r="AR2" s="122"/>
-      <c r="AS2" s="122"/>
-      <c r="AT2" s="122"/>
-      <c r="AU2" s="122"/>
-      <c r="AV2" s="122"/>
-      <c r="AW2" s="122"/>
-      <c r="AX2" s="122"/>
-      <c r="AY2" s="122"/>
-      <c r="AZ2" s="122"/>
-      <c r="BA2" s="122"/>
-      <c r="BB2" s="122"/>
-      <c r="BC2" s="122"/>
-      <c r="BD2" s="122"/>
-      <c r="BE2" s="123"/>
-      <c r="BF2" s="121" t="s">
+      <c r="AF2" s="128"/>
+      <c r="AG2" s="128"/>
+      <c r="AH2" s="128"/>
+      <c r="AI2" s="128"/>
+      <c r="AJ2" s="128"/>
+      <c r="AK2" s="128"/>
+      <c r="AL2" s="128"/>
+      <c r="AM2" s="128"/>
+      <c r="AN2" s="128"/>
+      <c r="AO2" s="128"/>
+      <c r="AP2" s="128"/>
+      <c r="AQ2" s="128"/>
+      <c r="AR2" s="128"/>
+      <c r="AS2" s="128"/>
+      <c r="AT2" s="128"/>
+      <c r="AU2" s="128"/>
+      <c r="AV2" s="128"/>
+      <c r="AW2" s="128"/>
+      <c r="AX2" s="128"/>
+      <c r="AY2" s="128"/>
+      <c r="AZ2" s="128"/>
+      <c r="BA2" s="128"/>
+      <c r="BB2" s="128"/>
+      <c r="BC2" s="128"/>
+      <c r="BD2" s="128"/>
+      <c r="BE2" s="129"/>
+      <c r="BF2" s="127" t="s">
         <v>31</v>
       </c>
-      <c r="BG2" s="122"/>
-      <c r="BH2" s="122"/>
-      <c r="BI2" s="122"/>
-      <c r="BJ2" s="122"/>
-      <c r="BK2" s="122"/>
-      <c r="BL2" s="122"/>
-      <c r="BM2" s="122"/>
-      <c r="BN2" s="122"/>
-      <c r="BO2" s="122"/>
-      <c r="BP2" s="122"/>
-      <c r="BQ2" s="122"/>
-      <c r="BR2" s="122"/>
-      <c r="BS2" s="122"/>
-      <c r="BT2" s="122"/>
-      <c r="BU2" s="122"/>
-      <c r="BV2" s="122"/>
-      <c r="BW2" s="122"/>
-      <c r="BX2" s="122"/>
-      <c r="BY2" s="122"/>
-      <c r="BZ2" s="122"/>
-      <c r="CA2" s="122"/>
-      <c r="CB2" s="122"/>
-      <c r="CC2" s="122"/>
-      <c r="CD2" s="122"/>
-      <c r="CE2" s="122"/>
-      <c r="CF2" s="123"/>
-      <c r="CG2" s="121" t="s">
+      <c r="BG2" s="128"/>
+      <c r="BH2" s="128"/>
+      <c r="BI2" s="128"/>
+      <c r="BJ2" s="128"/>
+      <c r="BK2" s="128"/>
+      <c r="BL2" s="128"/>
+      <c r="BM2" s="128"/>
+      <c r="BN2" s="128"/>
+      <c r="BO2" s="128"/>
+      <c r="BP2" s="128"/>
+      <c r="BQ2" s="128"/>
+      <c r="BR2" s="128"/>
+      <c r="BS2" s="128"/>
+      <c r="BT2" s="128"/>
+      <c r="BU2" s="128"/>
+      <c r="BV2" s="128"/>
+      <c r="BW2" s="128"/>
+      <c r="BX2" s="128"/>
+      <c r="BY2" s="128"/>
+      <c r="BZ2" s="128"/>
+      <c r="CA2" s="128"/>
+      <c r="CB2" s="128"/>
+      <c r="CC2" s="128"/>
+      <c r="CD2" s="128"/>
+      <c r="CE2" s="128"/>
+      <c r="CF2" s="129"/>
+      <c r="CG2" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="CH2" s="122"/>
-      <c r="CI2" s="122"/>
-      <c r="CJ2" s="122"/>
-      <c r="CK2" s="122"/>
-      <c r="CL2" s="122"/>
-      <c r="CM2" s="122"/>
-      <c r="CN2" s="122"/>
-      <c r="CO2" s="122"/>
-      <c r="CP2" s="122"/>
-      <c r="CQ2" s="122"/>
-      <c r="CR2" s="122"/>
-      <c r="CS2" s="122"/>
-      <c r="CT2" s="122"/>
-      <c r="CU2" s="122"/>
-      <c r="CV2" s="122"/>
-      <c r="CW2" s="122"/>
-      <c r="CX2" s="122"/>
-      <c r="CY2" s="122"/>
-      <c r="CZ2" s="122"/>
-      <c r="DA2" s="122"/>
-      <c r="DB2" s="122"/>
-      <c r="DC2" s="122"/>
-      <c r="DD2" s="122"/>
-      <c r="DE2" s="122"/>
-      <c r="DF2" s="122"/>
-      <c r="DG2" s="123"/>
-      <c r="DH2" s="121" t="s">
+      <c r="CH2" s="128"/>
+      <c r="CI2" s="128"/>
+      <c r="CJ2" s="128"/>
+      <c r="CK2" s="128"/>
+      <c r="CL2" s="128"/>
+      <c r="CM2" s="128"/>
+      <c r="CN2" s="128"/>
+      <c r="CO2" s="128"/>
+      <c r="CP2" s="128"/>
+      <c r="CQ2" s="128"/>
+      <c r="CR2" s="128"/>
+      <c r="CS2" s="128"/>
+      <c r="CT2" s="128"/>
+      <c r="CU2" s="128"/>
+      <c r="CV2" s="128"/>
+      <c r="CW2" s="128"/>
+      <c r="CX2" s="128"/>
+      <c r="CY2" s="128"/>
+      <c r="CZ2" s="128"/>
+      <c r="DA2" s="128"/>
+      <c r="DB2" s="128"/>
+      <c r="DC2" s="128"/>
+      <c r="DD2" s="128"/>
+      <c r="DE2" s="128"/>
+      <c r="DF2" s="128"/>
+      <c r="DG2" s="129"/>
+      <c r="DH2" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="DI2" s="122"/>
-      <c r="DJ2" s="122"/>
-      <c r="DK2" s="122"/>
-      <c r="DL2" s="122"/>
-      <c r="DM2" s="122"/>
-      <c r="DN2" s="122"/>
-      <c r="DO2" s="122"/>
-      <c r="DP2" s="122"/>
-      <c r="DQ2" s="122"/>
-      <c r="DR2" s="122"/>
-      <c r="DS2" s="122"/>
-      <c r="DT2" s="122"/>
-      <c r="DU2" s="122"/>
-      <c r="DV2" s="122"/>
-      <c r="DW2" s="122"/>
-      <c r="DX2" s="122"/>
-      <c r="DY2" s="122"/>
-      <c r="DZ2" s="122"/>
-      <c r="EA2" s="122"/>
-      <c r="EB2" s="122"/>
-      <c r="EC2" s="122"/>
-      <c r="ED2" s="122"/>
-      <c r="EE2" s="122"/>
-      <c r="EF2" s="122"/>
-      <c r="EG2" s="122"/>
-      <c r="EH2" s="123"/>
-      <c r="EI2" s="121" t="s">
+      <c r="DI2" s="128"/>
+      <c r="DJ2" s="128"/>
+      <c r="DK2" s="128"/>
+      <c r="DL2" s="128"/>
+      <c r="DM2" s="128"/>
+      <c r="DN2" s="128"/>
+      <c r="DO2" s="128"/>
+      <c r="DP2" s="128"/>
+      <c r="DQ2" s="128"/>
+      <c r="DR2" s="128"/>
+      <c r="DS2" s="128"/>
+      <c r="DT2" s="128"/>
+      <c r="DU2" s="128"/>
+      <c r="DV2" s="128"/>
+      <c r="DW2" s="128"/>
+      <c r="DX2" s="128"/>
+      <c r="DY2" s="128"/>
+      <c r="DZ2" s="128"/>
+      <c r="EA2" s="128"/>
+      <c r="EB2" s="128"/>
+      <c r="EC2" s="128"/>
+      <c r="ED2" s="128"/>
+      <c r="EE2" s="128"/>
+      <c r="EF2" s="128"/>
+      <c r="EG2" s="128"/>
+      <c r="EH2" s="129"/>
+      <c r="EI2" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="EJ2" s="122"/>
-      <c r="EK2" s="122"/>
-      <c r="EL2" s="122"/>
-      <c r="EM2" s="122"/>
-      <c r="EN2" s="122"/>
-      <c r="EO2" s="122"/>
-      <c r="EP2" s="122"/>
-      <c r="EQ2" s="122"/>
-      <c r="ER2" s="122"/>
-      <c r="ES2" s="122"/>
-      <c r="ET2" s="122"/>
-      <c r="EU2" s="122"/>
-      <c r="EV2" s="122"/>
-      <c r="EW2" s="122"/>
-      <c r="EX2" s="122"/>
-      <c r="EY2" s="122"/>
-      <c r="EZ2" s="122"/>
-      <c r="FA2" s="122"/>
-      <c r="FB2" s="122"/>
-      <c r="FC2" s="122"/>
-      <c r="FD2" s="122"/>
-      <c r="FE2" s="122"/>
-      <c r="FF2" s="122"/>
-      <c r="FG2" s="122"/>
-      <c r="FH2" s="122"/>
-      <c r="FI2" s="123"/>
-      <c r="FJ2" s="121" t="s">
+      <c r="EJ2" s="128"/>
+      <c r="EK2" s="128"/>
+      <c r="EL2" s="128"/>
+      <c r="EM2" s="128"/>
+      <c r="EN2" s="128"/>
+      <c r="EO2" s="128"/>
+      <c r="EP2" s="128"/>
+      <c r="EQ2" s="128"/>
+      <c r="ER2" s="128"/>
+      <c r="ES2" s="128"/>
+      <c r="ET2" s="128"/>
+      <c r="EU2" s="128"/>
+      <c r="EV2" s="128"/>
+      <c r="EW2" s="128"/>
+      <c r="EX2" s="128"/>
+      <c r="EY2" s="128"/>
+      <c r="EZ2" s="128"/>
+      <c r="FA2" s="128"/>
+      <c r="FB2" s="128"/>
+      <c r="FC2" s="128"/>
+      <c r="FD2" s="128"/>
+      <c r="FE2" s="128"/>
+      <c r="FF2" s="128"/>
+      <c r="FG2" s="128"/>
+      <c r="FH2" s="128"/>
+      <c r="FI2" s="129"/>
+      <c r="FJ2" s="127" t="s">
         <v>35</v>
       </c>
-      <c r="FK2" s="122"/>
-      <c r="FL2" s="122"/>
-      <c r="FM2" s="122"/>
-      <c r="FN2" s="122"/>
-      <c r="FO2" s="122"/>
-      <c r="FP2" s="122"/>
-      <c r="FQ2" s="122"/>
-      <c r="FR2" s="122"/>
-      <c r="FS2" s="122"/>
-      <c r="FT2" s="122"/>
-      <c r="FU2" s="122"/>
-      <c r="FV2" s="122"/>
-      <c r="FW2" s="122"/>
-      <c r="FX2" s="122"/>
-      <c r="FY2" s="122"/>
-      <c r="FZ2" s="122"/>
-      <c r="GA2" s="122"/>
-      <c r="GB2" s="122"/>
-      <c r="GC2" s="122"/>
-      <c r="GD2" s="122"/>
-      <c r="GE2" s="122"/>
-      <c r="GF2" s="122"/>
-      <c r="GG2" s="122"/>
-      <c r="GH2" s="122"/>
-      <c r="GI2" s="122"/>
-      <c r="GJ2" s="123"/>
-      <c r="GK2" s="121" t="s">
+      <c r="FK2" s="128"/>
+      <c r="FL2" s="128"/>
+      <c r="FM2" s="128"/>
+      <c r="FN2" s="128"/>
+      <c r="FO2" s="128"/>
+      <c r="FP2" s="128"/>
+      <c r="FQ2" s="128"/>
+      <c r="FR2" s="128"/>
+      <c r="FS2" s="128"/>
+      <c r="FT2" s="128"/>
+      <c r="FU2" s="128"/>
+      <c r="FV2" s="128"/>
+      <c r="FW2" s="128"/>
+      <c r="FX2" s="128"/>
+      <c r="FY2" s="128"/>
+      <c r="FZ2" s="128"/>
+      <c r="GA2" s="128"/>
+      <c r="GB2" s="128"/>
+      <c r="GC2" s="128"/>
+      <c r="GD2" s="128"/>
+      <c r="GE2" s="128"/>
+      <c r="GF2" s="128"/>
+      <c r="GG2" s="128"/>
+      <c r="GH2" s="128"/>
+      <c r="GI2" s="128"/>
+      <c r="GJ2" s="129"/>
+      <c r="GK2" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="GL2" s="122"/>
-      <c r="GM2" s="122"/>
-      <c r="GN2" s="122"/>
-      <c r="GO2" s="122"/>
-      <c r="GP2" s="122"/>
-      <c r="GQ2" s="122"/>
-      <c r="GR2" s="122"/>
-      <c r="GS2" s="122"/>
-      <c r="GT2" s="122"/>
-      <c r="GU2" s="122"/>
-      <c r="GV2" s="122"/>
-      <c r="GW2" s="122"/>
-      <c r="GX2" s="122"/>
-      <c r="GY2" s="122"/>
-      <c r="GZ2" s="122"/>
-      <c r="HA2" s="122"/>
-      <c r="HB2" s="122"/>
-      <c r="HC2" s="122"/>
-      <c r="HD2" s="122"/>
-      <c r="HE2" s="122"/>
-      <c r="HF2" s="122"/>
-      <c r="HG2" s="122"/>
-      <c r="HH2" s="122"/>
-      <c r="HI2" s="122"/>
-      <c r="HJ2" s="122"/>
-      <c r="HK2" s="123"/>
-      <c r="HL2" s="121" t="s">
+      <c r="GL2" s="128"/>
+      <c r="GM2" s="128"/>
+      <c r="GN2" s="128"/>
+      <c r="GO2" s="128"/>
+      <c r="GP2" s="128"/>
+      <c r="GQ2" s="128"/>
+      <c r="GR2" s="128"/>
+      <c r="GS2" s="128"/>
+      <c r="GT2" s="128"/>
+      <c r="GU2" s="128"/>
+      <c r="GV2" s="128"/>
+      <c r="GW2" s="128"/>
+      <c r="GX2" s="128"/>
+      <c r="GY2" s="128"/>
+      <c r="GZ2" s="128"/>
+      <c r="HA2" s="128"/>
+      <c r="HB2" s="128"/>
+      <c r="HC2" s="128"/>
+      <c r="HD2" s="128"/>
+      <c r="HE2" s="128"/>
+      <c r="HF2" s="128"/>
+      <c r="HG2" s="128"/>
+      <c r="HH2" s="128"/>
+      <c r="HI2" s="128"/>
+      <c r="HJ2" s="128"/>
+      <c r="HK2" s="129"/>
+      <c r="HL2" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="HM2" s="122"/>
-      <c r="HN2" s="122"/>
-      <c r="HO2" s="122"/>
-      <c r="HP2" s="122"/>
-      <c r="HQ2" s="122"/>
-      <c r="HR2" s="122"/>
-      <c r="HS2" s="122"/>
-      <c r="HT2" s="122"/>
-      <c r="HU2" s="122"/>
-      <c r="HV2" s="122"/>
-      <c r="HW2" s="122"/>
-      <c r="HX2" s="122"/>
-      <c r="HY2" s="122"/>
-      <c r="HZ2" s="122"/>
-      <c r="IA2" s="122"/>
-      <c r="IB2" s="122"/>
-      <c r="IC2" s="122"/>
-      <c r="ID2" s="122"/>
-      <c r="IE2" s="122"/>
-      <c r="IF2" s="122"/>
-      <c r="IG2" s="122"/>
-      <c r="IH2" s="122"/>
-      <c r="II2" s="122"/>
-      <c r="IJ2" s="122"/>
-      <c r="IK2" s="122"/>
-      <c r="IL2" s="123"/>
-      <c r="IM2" s="121" t="s">
+      <c r="HM2" s="128"/>
+      <c r="HN2" s="128"/>
+      <c r="HO2" s="128"/>
+      <c r="HP2" s="128"/>
+      <c r="HQ2" s="128"/>
+      <c r="HR2" s="128"/>
+      <c r="HS2" s="128"/>
+      <c r="HT2" s="128"/>
+      <c r="HU2" s="128"/>
+      <c r="HV2" s="128"/>
+      <c r="HW2" s="128"/>
+      <c r="HX2" s="128"/>
+      <c r="HY2" s="128"/>
+      <c r="HZ2" s="128"/>
+      <c r="IA2" s="128"/>
+      <c r="IB2" s="128"/>
+      <c r="IC2" s="128"/>
+      <c r="ID2" s="128"/>
+      <c r="IE2" s="128"/>
+      <c r="IF2" s="128"/>
+      <c r="IG2" s="128"/>
+      <c r="IH2" s="128"/>
+      <c r="II2" s="128"/>
+      <c r="IJ2" s="128"/>
+      <c r="IK2" s="128"/>
+      <c r="IL2" s="129"/>
+      <c r="IM2" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="IN2" s="122"/>
-      <c r="IO2" s="122"/>
-      <c r="IP2" s="122"/>
-      <c r="IQ2" s="122"/>
-      <c r="IR2" s="122"/>
-      <c r="IS2" s="122"/>
-      <c r="IT2" s="122"/>
-      <c r="IU2" s="122"/>
-      <c r="IV2" s="122"/>
-      <c r="IW2" s="122"/>
-      <c r="IX2" s="122"/>
-      <c r="IY2" s="122"/>
-      <c r="IZ2" s="122"/>
-      <c r="JA2" s="122"/>
-      <c r="JB2" s="122"/>
-      <c r="JC2" s="122"/>
-      <c r="JD2" s="122"/>
-      <c r="JE2" s="122"/>
-      <c r="JF2" s="122"/>
-      <c r="JG2" s="122"/>
-      <c r="JH2" s="122"/>
-      <c r="JI2" s="122"/>
-      <c r="JJ2" s="122"/>
-      <c r="JK2" s="122"/>
-      <c r="JL2" s="122"/>
-      <c r="JM2" s="123"/>
-      <c r="JN2" s="121" t="s">
+      <c r="IN2" s="128"/>
+      <c r="IO2" s="128"/>
+      <c r="IP2" s="128"/>
+      <c r="IQ2" s="128"/>
+      <c r="IR2" s="128"/>
+      <c r="IS2" s="128"/>
+      <c r="IT2" s="128"/>
+      <c r="IU2" s="128"/>
+      <c r="IV2" s="128"/>
+      <c r="IW2" s="128"/>
+      <c r="IX2" s="128"/>
+      <c r="IY2" s="128"/>
+      <c r="IZ2" s="128"/>
+      <c r="JA2" s="128"/>
+      <c r="JB2" s="128"/>
+      <c r="JC2" s="128"/>
+      <c r="JD2" s="128"/>
+      <c r="JE2" s="128"/>
+      <c r="JF2" s="128"/>
+      <c r="JG2" s="128"/>
+      <c r="JH2" s="128"/>
+      <c r="JI2" s="128"/>
+      <c r="JJ2" s="128"/>
+      <c r="JK2" s="128"/>
+      <c r="JL2" s="128"/>
+      <c r="JM2" s="129"/>
+      <c r="JN2" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="JO2" s="122"/>
-      <c r="JP2" s="122"/>
-      <c r="JQ2" s="122"/>
-      <c r="JR2" s="122"/>
-      <c r="JS2" s="122"/>
-      <c r="JT2" s="122"/>
-      <c r="JU2" s="122"/>
-      <c r="JV2" s="122"/>
-      <c r="JW2" s="122"/>
-      <c r="JX2" s="122"/>
-      <c r="JY2" s="122"/>
-      <c r="JZ2" s="122"/>
-      <c r="KA2" s="122"/>
-      <c r="KB2" s="122"/>
-      <c r="KC2" s="122"/>
-      <c r="KD2" s="122"/>
-      <c r="KE2" s="122"/>
-      <c r="KF2" s="122"/>
-      <c r="KG2" s="122"/>
-      <c r="KH2" s="122"/>
-      <c r="KI2" s="122"/>
-      <c r="KJ2" s="122"/>
-      <c r="KK2" s="122"/>
-      <c r="KL2" s="122"/>
-      <c r="KM2" s="122"/>
-      <c r="KN2" s="123"/>
-      <c r="KO2" s="121" t="s">
+      <c r="JO2" s="128"/>
+      <c r="JP2" s="128"/>
+      <c r="JQ2" s="128"/>
+      <c r="JR2" s="128"/>
+      <c r="JS2" s="128"/>
+      <c r="JT2" s="128"/>
+      <c r="JU2" s="128"/>
+      <c r="JV2" s="128"/>
+      <c r="JW2" s="128"/>
+      <c r="JX2" s="128"/>
+      <c r="JY2" s="128"/>
+      <c r="JZ2" s="128"/>
+      <c r="KA2" s="128"/>
+      <c r="KB2" s="128"/>
+      <c r="KC2" s="128"/>
+      <c r="KD2" s="128"/>
+      <c r="KE2" s="128"/>
+      <c r="KF2" s="128"/>
+      <c r="KG2" s="128"/>
+      <c r="KH2" s="128"/>
+      <c r="KI2" s="128"/>
+      <c r="KJ2" s="128"/>
+      <c r="KK2" s="128"/>
+      <c r="KL2" s="128"/>
+      <c r="KM2" s="128"/>
+      <c r="KN2" s="129"/>
+      <c r="KO2" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="KP2" s="122"/>
-      <c r="KQ2" s="122"/>
-      <c r="KR2" s="122"/>
-      <c r="KS2" s="122"/>
-      <c r="KT2" s="122"/>
-      <c r="KU2" s="122"/>
-      <c r="KV2" s="122"/>
-      <c r="KW2" s="122"/>
-      <c r="KX2" s="122"/>
-      <c r="KY2" s="122"/>
-      <c r="KZ2" s="122"/>
-      <c r="LA2" s="122"/>
-      <c r="LB2" s="122"/>
-      <c r="LC2" s="122"/>
-      <c r="LD2" s="122"/>
-      <c r="LE2" s="122"/>
-      <c r="LF2" s="122"/>
-      <c r="LG2" s="122"/>
-      <c r="LH2" s="122"/>
-      <c r="LI2" s="122"/>
-      <c r="LJ2" s="122"/>
-      <c r="LK2" s="122"/>
-      <c r="LL2" s="122"/>
-      <c r="LM2" s="122"/>
-      <c r="LN2" s="122"/>
-      <c r="LO2" s="123"/>
-      <c r="LP2" s="121" t="s">
+      <c r="KP2" s="128"/>
+      <c r="KQ2" s="128"/>
+      <c r="KR2" s="128"/>
+      <c r="KS2" s="128"/>
+      <c r="KT2" s="128"/>
+      <c r="KU2" s="128"/>
+      <c r="KV2" s="128"/>
+      <c r="KW2" s="128"/>
+      <c r="KX2" s="128"/>
+      <c r="KY2" s="128"/>
+      <c r="KZ2" s="128"/>
+      <c r="LA2" s="128"/>
+      <c r="LB2" s="128"/>
+      <c r="LC2" s="128"/>
+      <c r="LD2" s="128"/>
+      <c r="LE2" s="128"/>
+      <c r="LF2" s="128"/>
+      <c r="LG2" s="128"/>
+      <c r="LH2" s="128"/>
+      <c r="LI2" s="128"/>
+      <c r="LJ2" s="128"/>
+      <c r="LK2" s="128"/>
+      <c r="LL2" s="128"/>
+      <c r="LM2" s="128"/>
+      <c r="LN2" s="128"/>
+      <c r="LO2" s="129"/>
+      <c r="LP2" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="LQ2" s="122"/>
-      <c r="LR2" s="122"/>
-      <c r="LS2" s="122"/>
-      <c r="LT2" s="122"/>
-      <c r="LU2" s="122"/>
-      <c r="LV2" s="122"/>
-      <c r="LW2" s="122"/>
-      <c r="LX2" s="122"/>
-      <c r="LY2" s="122"/>
-      <c r="LZ2" s="122"/>
-      <c r="MA2" s="122"/>
-      <c r="MB2" s="122"/>
-      <c r="MC2" s="122"/>
-      <c r="MD2" s="122"/>
-      <c r="ME2" s="122"/>
-      <c r="MF2" s="122"/>
-      <c r="MG2" s="122"/>
-      <c r="MH2" s="122"/>
-      <c r="MI2" s="122"/>
-      <c r="MJ2" s="122"/>
-      <c r="MK2" s="122"/>
-      <c r="ML2" s="122"/>
-      <c r="MM2" s="122"/>
-      <c r="MN2" s="122"/>
-      <c r="MO2" s="122"/>
-      <c r="MP2" s="123"/>
-      <c r="MQ2" s="121" t="s">
+      <c r="LQ2" s="128"/>
+      <c r="LR2" s="128"/>
+      <c r="LS2" s="128"/>
+      <c r="LT2" s="128"/>
+      <c r="LU2" s="128"/>
+      <c r="LV2" s="128"/>
+      <c r="LW2" s="128"/>
+      <c r="LX2" s="128"/>
+      <c r="LY2" s="128"/>
+      <c r="LZ2" s="128"/>
+      <c r="MA2" s="128"/>
+      <c r="MB2" s="128"/>
+      <c r="MC2" s="128"/>
+      <c r="MD2" s="128"/>
+      <c r="ME2" s="128"/>
+      <c r="MF2" s="128"/>
+      <c r="MG2" s="128"/>
+      <c r="MH2" s="128"/>
+      <c r="MI2" s="128"/>
+      <c r="MJ2" s="128"/>
+      <c r="MK2" s="128"/>
+      <c r="ML2" s="128"/>
+      <c r="MM2" s="128"/>
+      <c r="MN2" s="128"/>
+      <c r="MO2" s="128"/>
+      <c r="MP2" s="129"/>
+      <c r="MQ2" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="MR2" s="122"/>
-      <c r="MS2" s="122"/>
-      <c r="MT2" s="122"/>
-      <c r="MU2" s="122"/>
-      <c r="MV2" s="122"/>
-      <c r="MW2" s="122"/>
-      <c r="MX2" s="122"/>
-      <c r="MY2" s="122"/>
-      <c r="MZ2" s="122"/>
-      <c r="NA2" s="122"/>
-      <c r="NB2" s="122"/>
-      <c r="NC2" s="122"/>
-      <c r="ND2" s="122"/>
-      <c r="NE2" s="122"/>
-      <c r="NF2" s="122"/>
-      <c r="NG2" s="122"/>
-      <c r="NH2" s="122"/>
-      <c r="NI2" s="122"/>
-      <c r="NJ2" s="122"/>
-      <c r="NK2" s="122"/>
-      <c r="NL2" s="122"/>
-      <c r="NM2" s="122"/>
-      <c r="NN2" s="122"/>
-      <c r="NO2" s="122"/>
-      <c r="NP2" s="122"/>
-      <c r="NQ2" s="123"/>
-      <c r="NR2" s="121" t="s">
+      <c r="MR2" s="128"/>
+      <c r="MS2" s="128"/>
+      <c r="MT2" s="128"/>
+      <c r="MU2" s="128"/>
+      <c r="MV2" s="128"/>
+      <c r="MW2" s="128"/>
+      <c r="MX2" s="128"/>
+      <c r="MY2" s="128"/>
+      <c r="MZ2" s="128"/>
+      <c r="NA2" s="128"/>
+      <c r="NB2" s="128"/>
+      <c r="NC2" s="128"/>
+      <c r="ND2" s="128"/>
+      <c r="NE2" s="128"/>
+      <c r="NF2" s="128"/>
+      <c r="NG2" s="128"/>
+      <c r="NH2" s="128"/>
+      <c r="NI2" s="128"/>
+      <c r="NJ2" s="128"/>
+      <c r="NK2" s="128"/>
+      <c r="NL2" s="128"/>
+      <c r="NM2" s="128"/>
+      <c r="NN2" s="128"/>
+      <c r="NO2" s="128"/>
+      <c r="NP2" s="128"/>
+      <c r="NQ2" s="129"/>
+      <c r="NR2" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="NS2" s="122"/>
-      <c r="NT2" s="122"/>
-      <c r="NU2" s="122"/>
-      <c r="NV2" s="122"/>
-      <c r="NW2" s="122"/>
-      <c r="NX2" s="122"/>
-      <c r="NY2" s="122"/>
-      <c r="NZ2" s="122"/>
-      <c r="OA2" s="122"/>
-      <c r="OB2" s="122"/>
-      <c r="OC2" s="122"/>
-      <c r="OD2" s="122"/>
-      <c r="OE2" s="122"/>
-      <c r="OF2" s="122"/>
-      <c r="OG2" s="122"/>
-      <c r="OH2" s="122"/>
-      <c r="OI2" s="122"/>
-      <c r="OJ2" s="122"/>
-      <c r="OK2" s="122"/>
-      <c r="OL2" s="122"/>
-      <c r="OM2" s="122"/>
-      <c r="ON2" s="122"/>
-      <c r="OO2" s="122"/>
-      <c r="OP2" s="122"/>
-      <c r="OQ2" s="122"/>
-      <c r="OR2" s="123"/>
-      <c r="OS2" s="121" t="s">
+      <c r="NS2" s="128"/>
+      <c r="NT2" s="128"/>
+      <c r="NU2" s="128"/>
+      <c r="NV2" s="128"/>
+      <c r="NW2" s="128"/>
+      <c r="NX2" s="128"/>
+      <c r="NY2" s="128"/>
+      <c r="NZ2" s="128"/>
+      <c r="OA2" s="128"/>
+      <c r="OB2" s="128"/>
+      <c r="OC2" s="128"/>
+      <c r="OD2" s="128"/>
+      <c r="OE2" s="128"/>
+      <c r="OF2" s="128"/>
+      <c r="OG2" s="128"/>
+      <c r="OH2" s="128"/>
+      <c r="OI2" s="128"/>
+      <c r="OJ2" s="128"/>
+      <c r="OK2" s="128"/>
+      <c r="OL2" s="128"/>
+      <c r="OM2" s="128"/>
+      <c r="ON2" s="128"/>
+      <c r="OO2" s="128"/>
+      <c r="OP2" s="128"/>
+      <c r="OQ2" s="128"/>
+      <c r="OR2" s="129"/>
+      <c r="OS2" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="OT2" s="122"/>
-      <c r="OU2" s="122"/>
-      <c r="OV2" s="122"/>
-      <c r="OW2" s="122"/>
-      <c r="OX2" s="122"/>
-      <c r="OY2" s="122"/>
-      <c r="OZ2" s="122"/>
-      <c r="PA2" s="122"/>
-      <c r="PB2" s="122"/>
-      <c r="PC2" s="122"/>
-      <c r="PD2" s="122"/>
-      <c r="PE2" s="122"/>
-      <c r="PF2" s="122"/>
-      <c r="PG2" s="122"/>
-      <c r="PH2" s="122"/>
-      <c r="PI2" s="122"/>
-      <c r="PJ2" s="122"/>
-      <c r="PK2" s="122"/>
-      <c r="PL2" s="122"/>
-      <c r="PM2" s="122"/>
-      <c r="PN2" s="122"/>
-      <c r="PO2" s="122"/>
-      <c r="PP2" s="122"/>
-      <c r="PQ2" s="122"/>
-      <c r="PR2" s="122"/>
-      <c r="PS2" s="123"/>
+      <c r="OT2" s="128"/>
+      <c r="OU2" s="128"/>
+      <c r="OV2" s="128"/>
+      <c r="OW2" s="128"/>
+      <c r="OX2" s="128"/>
+      <c r="OY2" s="128"/>
+      <c r="OZ2" s="128"/>
+      <c r="PA2" s="128"/>
+      <c r="PB2" s="128"/>
+      <c r="PC2" s="128"/>
+      <c r="PD2" s="128"/>
+      <c r="PE2" s="128"/>
+      <c r="PF2" s="128"/>
+      <c r="PG2" s="128"/>
+      <c r="PH2" s="128"/>
+      <c r="PI2" s="128"/>
+      <c r="PJ2" s="128"/>
+      <c r="PK2" s="128"/>
+      <c r="PL2" s="128"/>
+      <c r="PM2" s="128"/>
+      <c r="PN2" s="128"/>
+      <c r="PO2" s="128"/>
+      <c r="PP2" s="128"/>
+      <c r="PQ2" s="128"/>
+      <c r="PR2" s="128"/>
+      <c r="PS2" s="129"/>
     </row>
     <row r="3" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85"/>
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="132" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="30">
@@ -4479,7 +4494,7 @@
     </row>
     <row r="4" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="85"/>
-      <c r="B4" s="127"/>
+      <c r="B4" s="133"/>
       <c r="C4" s="44">
         <v>0</v>
       </c>
@@ -4917,7 +4932,7 @@
       <c r="PS4" s="95"/>
     </row>
     <row r="5" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="128" t="str">
+      <c r="B5" s="134" t="str">
         <f>Donnees!$C$21</f>
         <v>Rédaction CDC</v>
       </c>
@@ -5358,7 +5373,7 @@
       <c r="PS5" s="90"/>
     </row>
     <row r="6" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="125"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="97">
         <v>0</v>
       </c>
@@ -5796,7 +5811,7 @@
       <c r="PS6" s="95"/>
     </row>
     <row r="7" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="124" t="str">
+      <c r="B7" s="130" t="str">
         <f>Donnees!$C$22</f>
         <v>Mise en place Trello</v>
       </c>
@@ -6237,7 +6252,7 @@
       <c r="PS7" s="90"/>
     </row>
     <row r="8" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="125"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="97">
         <v>0</v>
       </c>
@@ -6675,7 +6690,7 @@
       <c r="PS8" s="95"/>
     </row>
     <row r="9" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="124" t="str">
+      <c r="B9" s="130" t="str">
         <f>Donnees!$C$23</f>
         <v>Mise en place GitKraken</v>
       </c>
@@ -7116,7 +7131,7 @@
       <c r="PS9" s="90"/>
     </row>
     <row r="10" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="125"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="97">
         <v>0</v>
       </c>
@@ -7554,7 +7569,7 @@
       <c r="PS10" s="95"/>
     </row>
     <row r="11" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="124" t="str">
+      <c r="B11" s="130" t="str">
         <f>Donnees!$C$24</f>
         <v>Mise à jour Trello</v>
       </c>
@@ -7995,7 +8010,7 @@
       <c r="PS11" s="90"/>
     </row>
     <row r="12" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="125"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="97">
         <v>0</v>
       </c>
@@ -8433,7 +8448,7 @@
       <c r="PS12" s="95"/>
     </row>
     <row r="13" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="124" t="str">
+      <c r="B13" s="130" t="str">
         <f>Donnees!$C$25</f>
         <v>Mise à jour GitKraken</v>
       </c>
@@ -8874,7 +8889,7 @@
       <c r="PS13" s="90"/>
     </row>
     <row r="14" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="125"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="97">
         <v>0</v>
       </c>
@@ -9312,7 +9327,7 @@
       <c r="PS14" s="95"/>
     </row>
     <row r="15" spans="1:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="124" t="str">
+      <c r="B15" s="130" t="str">
         <f>Donnees!$C$26</f>
         <v>Recherches</v>
       </c>
@@ -9754,7 +9769,7 @@
     </row>
     <row r="16" spans="1:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
-      <c r="B16" s="125"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="97">
         <v>0</v>
       </c>
@@ -10192,7 +10207,7 @@
       <c r="PS16" s="95"/>
     </row>
     <row r="17" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="124" t="str">
+      <c r="B17" s="130" t="str">
         <f>Donnees!$C$27</f>
         <v>Création plannif + JDT</v>
       </c>
@@ -10633,7 +10648,7 @@
       <c r="PS17" s="90"/>
     </row>
     <row r="18" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="125"/>
+      <c r="B18" s="131"/>
       <c r="C18" s="97">
         <v>0</v>
       </c>
@@ -11071,7 +11086,7 @@
       <c r="PS18" s="95"/>
     </row>
     <row r="19" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="124" t="str">
+      <c r="B19" s="130" t="str">
         <f>Donnees!$C$28</f>
         <v>Mise à jour du JDT</v>
       </c>
@@ -11512,7 +11527,7 @@
       <c r="PS19" s="90"/>
     </row>
     <row r="20" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="125"/>
+      <c r="B20" s="131"/>
       <c r="C20" s="97">
         <v>0</v>
       </c>
@@ -11950,7 +11965,7 @@
       <c r="PS20" s="95"/>
     </row>
     <row r="21" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="124" t="str">
+      <c r="B21" s="130" t="str">
         <f>Donnees!$C$29</f>
         <v>Daily Scrum</v>
       </c>
@@ -12391,7 +12406,7 @@
       <c r="PS21" s="90"/>
     </row>
     <row r="22" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="125"/>
+      <c r="B22" s="131"/>
       <c r="C22" s="97">
         <v>0</v>
       </c>
@@ -12829,7 +12844,7 @@
       <c r="PS22" s="95"/>
     </row>
     <row r="23" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="124" t="str">
+      <c r="B23" s="130" t="str">
         <f>Donnees!$C$30</f>
         <v>HTML</v>
       </c>
@@ -13270,7 +13285,7 @@
       <c r="PS23" s="90"/>
     </row>
     <row r="24" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="125"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="97">
         <v>0</v>
       </c>
@@ -13708,7 +13723,7 @@
       <c r="PS24" s="95"/>
     </row>
     <row r="25" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="124" t="str">
+      <c r="B25" s="130" t="str">
         <f>Donnees!$C$31</f>
         <v>Base de donnée</v>
       </c>
@@ -14149,7 +14164,7 @@
       <c r="PS25" s="90"/>
     </row>
     <row r="26" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="125"/>
+      <c r="B26" s="131"/>
       <c r="C26" s="97">
         <v>0</v>
       </c>
@@ -14587,7 +14602,7 @@
       <c r="PS26" s="95"/>
     </row>
     <row r="27" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="124" t="str">
+      <c r="B27" s="130" t="str">
         <f>Donnees!$C$32</f>
         <v>PHP</v>
       </c>
@@ -15028,7 +15043,7 @@
       <c r="PS27" s="90"/>
     </row>
     <row r="28" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="125"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="97">
         <v>0</v>
       </c>
@@ -15466,7 +15481,7 @@
       <c r="PS28" s="95"/>
     </row>
     <row r="29" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="124" t="str">
+      <c r="B29" s="130" t="str">
         <f>Donnees!$C$33</f>
         <v>Typo3</v>
       </c>
@@ -15907,7 +15922,7 @@
       <c r="PS29" s="90"/>
     </row>
     <row r="30" spans="2:435" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="125"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="97">
         <v>0</v>
       </c>
@@ -16345,7 +16360,7 @@
       <c r="PS30" s="95"/>
     </row>
     <row r="31" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="124" t="str">
+      <c r="B31" s="130" t="str">
         <f>Donnees!$C$34</f>
         <v>Création jeu flash</v>
       </c>
@@ -16786,7 +16801,7 @@
       <c r="PS31" s="90"/>
     </row>
     <row r="32" spans="2:435" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="125"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="97">
         <v>0</v>
       </c>
@@ -18188,7 +18203,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="132" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="30">
@@ -18197,7 +18212,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
-      <c r="B4" s="129"/>
+      <c r="B4" s="135"/>
       <c r="C4" s="44">
         <v>0</v>
       </c>
@@ -20807,8 +20822,8 @@
   </sheetPr>
   <dimension ref="A1:I298"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A157" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A175" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22588,21 +22603,21 @@
       <c r="D169" s="14"/>
     </row>
     <row r="170" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A170" s="133"/>
-      <c r="B170" s="134"/>
-      <c r="C170" s="135" t="s">
+      <c r="A170" s="122"/>
+      <c r="B170" s="123"/>
+      <c r="C170" s="124" t="s">
         <v>78</v>
       </c>
       <c r="D170" s="14"/>
     </row>
     <row r="171" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A171" s="130" t="s">
+      <c r="A171" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="B171" s="131">
+      <c r="B171" s="120">
         <v>2</v>
       </c>
-      <c r="C171" s="132" t="s">
+      <c r="C171" s="121" t="s">
         <v>131</v>
       </c>
       <c r="D171" s="108" t="s">
@@ -22733,39 +22748,71 @@
       </c>
     </row>
     <row r="186" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A186" s="9"/>
-      <c r="B186" s="8"/>
-      <c r="C186" s="13"/>
+      <c r="A186" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B186" s="8">
+        <v>1</v>
+      </c>
+      <c r="C186" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="D186" s="13"/>
     </row>
-    <row r="187" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A187" s="5"/>
-      <c r="B187" s="6"/>
-      <c r="C187" s="14"/>
+    <row r="187" spans="1:4" ht="27" x14ac:dyDescent="0.2">
+      <c r="A187" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B187" s="6">
+        <v>13</v>
+      </c>
+      <c r="C187" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="D187" s="14"/>
     </row>
     <row r="188" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A188" s="5"/>
-      <c r="B188" s="6"/>
-      <c r="C188" s="14"/>
+      <c r="A188" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B188" s="6">
+        <v>1</v>
+      </c>
+      <c r="C188" s="14" t="s">
+        <v>134</v>
+      </c>
       <c r="D188" s="14"/>
     </row>
     <row r="189" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A189" s="5"/>
       <c r="B189" s="6"/>
-      <c r="C189" s="14"/>
+      <c r="C189" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="D189" s="14"/>
     </row>
-    <row r="190" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A190" s="5"/>
-      <c r="B190" s="6"/>
-      <c r="C190" s="14"/>
+    <row r="190" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A190" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B190" s="6">
+        <v>5</v>
+      </c>
+      <c r="C190" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="D190" s="14"/>
     </row>
     <row r="191" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A191" s="5"/>
-      <c r="B191" s="6"/>
-      <c r="C191" s="14"/>
+      <c r="A191" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" s="6">
+        <v>7</v>
+      </c>
+      <c r="C191" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -22828,7 +22875,7 @@
       </c>
       <c r="B201" s="76">
         <f>SUM(B186:B200)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C201" s="107" t="s">
         <v>45</v>
@@ -22989,7 +23036,7 @@
         <v>23</v>
       </c>
       <c r="D222" s="82">
-        <v>42968</v>
+        <v>42913</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>